<commit_message>
- force LocatorHelper.findBy to be Not-Nullable - honor `nexial.browser.forceJSClick` so that if it is set to `false` then Nexial will not automate `click` via JavaScript - enable web element highlight during the execution of `assert`* commands - supports replacing multiple `(empty)`, `(blank)`, `(tab)` and `(eol)` with the appropriate values
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-03.data.xlsx
+++ b/artifact/data/web-03.data.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10723"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10806"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F3BC61-DCD0-0141-8A46-7A2FAD259129}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70575901-2ACA-9741-A3C0-DC0AB350D330}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="18100" windowHeight="9900" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="10500" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
-    <sheet name="locators" sheetId="3" r:id="rId2"/>
+    <sheet name="locators-class" sheetId="3" r:id="rId2"/>
+    <sheet name="locators-css" sheetId="4" r:id="rId3"/>
+    <sheet name="locators-id" sheetId="5" r:id="rId4"/>
+    <sheet name="locators-tag" sheetId="6" r:id="rId5"/>
+    <sheet name="locators-name" sheetId="7" r:id="rId6"/>
+    <sheet name="locators-xpath" sheetId="8" r:id="rId7"/>
+    <sheet name="locators-link" sheetId="9" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -50,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="123">
   <si>
     <t>true</t>
   </si>
@@ -167,13 +173,271 @@
   </si>
   <si>
     <t>aut : references : file</t>
+  </si>
+  <si>
+    <t>loc : class : mbox</t>
+  </si>
+  <si>
+    <t>aut : mbox : count</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>class=mbox-text</t>
+  </si>
+  <si>
+    <t>loc : css : portalLinks</t>
+  </si>
+  <si>
+    <t>css=div.noprint a.mw-redirect</t>
+  </si>
+  <si>
+    <t>loc : css : portalLinks2</t>
+  </si>
+  <si>
+    <t>css=div.noprint a:not([href*='.jpg']):not([href*='.gif'])</t>
+  </si>
+  <si>
+    <t>aut : portal : text</t>
+  </si>
+  <si>
+    <t>aut : portal2 : text</t>
+  </si>
+  <si>
+    <t>aut : portal : count</t>
+  </si>
+  <si>
+    <t>aut : portal2 : count</t>
+  </si>
+  <si>
+    <t>$(array|length|${aut : portal : text})</t>
+  </si>
+  <si>
+    <t>$(array|length|${aut : portal2 : text})</t>
+  </si>
+  <si>
+    <t>Computer Science portal,Computing portal</t>
+  </si>
+  <si>
+    <t>Computer Science portal,Computing portal,Computer programming portal</t>
+  </si>
+  <si>
+    <t>aut : usernameStatus : id</t>
+  </si>
+  <si>
+    <t>aut : password : id</t>
+  </si>
+  <si>
+    <t>aut : passwordStatus : id</t>
+  </si>
+  <si>
+    <t>aut : phone : id</t>
+  </si>
+  <si>
+    <t>aut : phoneStatus : id</t>
+  </si>
+  <si>
+    <t>Please enter a valid phone number</t>
+  </si>
+  <si>
+    <t>Weak password</t>
+  </si>
+  <si>
+    <t>Username is available!</t>
+  </si>
+  <si>
+    <t>id=username</t>
+  </si>
+  <si>
+    <t>id=usernameStatus</t>
+  </si>
+  <si>
+    <t>id=password</t>
+  </si>
+  <si>
+    <t>id=passwordStatus</t>
+  </si>
+  <si>
+    <t>id=phone</t>
+  </si>
+  <si>
+    <t>id=phoneStatus</t>
+  </si>
+  <si>
+    <t>aut : usernameStatus : availalable</t>
+  </si>
+  <si>
+    <t>aut : passwordStatus : weak</t>
+  </si>
+  <si>
+    <t>aut : phoneStatus : notValid</t>
+  </si>
+  <si>
+    <t>https://www.quackit.com/html/html_editors/scratchpad/preview.cfm?example=/html/codes/html_form_code_right_aligned_labels</t>
+  </si>
+  <si>
+    <t>aut : username : name</t>
+  </si>
+  <si>
+    <t>https://simfatic.com/form_gallary/contact_us/contact_us.php</t>
+  </si>
+  <si>
+    <t>id=Name</t>
+  </si>
+  <si>
+    <t>aut : heading : text</t>
+  </si>
+  <si>
+    <t>Contact us</t>
+  </si>
+  <si>
+    <t>id=TextBlock</t>
+  </si>
+  <si>
+    <t>aut : nameLabel : loc</t>
+  </si>
+  <si>
+    <t>aut : email : loc</t>
+  </si>
+  <si>
+    <t>aut : emailLabel : loc</t>
+  </si>
+  <si>
+    <t>aut : message : loc</t>
+  </si>
+  <si>
+    <t>aut : messageLabel : loc</t>
+  </si>
+  <si>
+    <t>aut : heading : loc</t>
+  </si>
+  <si>
+    <t>id=Email</t>
+  </si>
+  <si>
+    <t>id=TextBlock1</t>
+  </si>
+  <si>
+    <t>aut : emailLabel : text</t>
+  </si>
+  <si>
+    <t>Email*</t>
+  </si>
+  <si>
+    <t>aut : nameLabel : text</t>
+  </si>
+  <si>
+    <t>Name*</t>
+  </si>
+  <si>
+    <t>aut : messageLabel : text</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>id=Message</t>
+  </si>
+  <si>
+    <t>id=TextBlock2</t>
+  </si>
+  <si>
+    <t>aut : submit : loc</t>
+  </si>
+  <si>
+    <t>aut : submit : text</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>id=contact_us_Submit_img</t>
+  </si>
+  <si>
+    <t>aut : submit : img</t>
+  </si>
+  <si>
+    <t>aut : name : loc</t>
+  </si>
+  <si>
+    <t>aut : error : loc</t>
+  </si>
+  <si>
+    <t>class=sfm_float_error_box</t>
+  </si>
+  <si>
+    <t>aut : error : tc1 : alt</t>
+  </si>
+  <si>
+    <t>Name,Email</t>
+  </si>
+  <si>
+    <t>aut : error : tc1</t>
+  </si>
+  <si>
+    <t>aut : errorClose : loc</t>
+  </si>
+  <si>
+    <t>class=sfm_close_box</t>
+  </si>
+  <si>
+    <t>Please fill in Name
+X,Please fill in Email
+X</t>
+  </si>
+  <si>
+    <t>id=heading</t>
+  </si>
+  <si>
+    <t>nexial.highlight</t>
+  </si>
+  <si>
+    <t>nexial.highlightWaitMs</t>
+  </si>
+  <si>
+    <t>aut : error : tc2</t>
+  </si>
+  <si>
+    <t>aut : error : tc3</t>
+  </si>
+  <si>
+    <t>The input for Email should be a valid email value
+X</t>
+  </si>
+  <si>
+    <t>aut : error : tc4</t>
+  </si>
+  <si>
+    <t>aut : success : text</t>
+  </si>
+  <si>
+    <t>Thank You!
+The form is successfully submitted. 
+Thank you very much for your input.</t>
+  </si>
+  <si>
+    <t>Please fill in Message
+X</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>nexial.browser.forceJSClick</t>
+  </si>
+  <si>
+    <t>aut : error : tc5</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/web-03-submit.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -219,6 +483,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -261,7 +531,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -285,6 +555,14 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -295,7 +573,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="104">
     <dxf>
       <font>
         <b val="0"/>
@@ -321,6 +599,1194 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -743,15 +2209,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA9"/>
+  <dimension ref="A1:AAA21"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="115" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="34" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="27" style="2" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
@@ -770,47 +2236,47 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="HA3" s="4"/>
-      <c r="AAA3" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -820,47 +2286,120 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
     <row r="9" spans="1:703">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
+    <row r="10" spans="1:703">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:703">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:703">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:703">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:703">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:703">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:703">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+  <conditionalFormatting sqref="A1 A3:A9 A22:A1048576">
+    <cfRule type="beginsWith" dxfId="103" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="102" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="9" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="101" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
+  <conditionalFormatting sqref="B1 B3:B9 B22:B1048576">
+    <cfRule type="expression" dxfId="100" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="99" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="beginsWith" dxfId="98" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="97" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="96" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="expression" dxfId="95" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="94" priority="5">
+      <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -870,10 +2409,841 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02992098-561F-1944-A340-34CB95735B3B}">
-  <dimension ref="A1:AAA13"/>
+  <dimension ref="A1:AAA9"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="88.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703">
+      <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="HA3" s="4"/>
+      <c r="AAA3" s="5"/>
+    </row>
+    <row r="4" spans="1:703">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <sortState ref="A1:B9">
+    <sortCondition ref="A1:A9"/>
+  </sortState>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="beginsWith" dxfId="93" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="92" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="91" priority="10" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="expression" dxfId="90" priority="11" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="89" priority="12">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CC5913-9CC1-104B-A93C-2AE9134DFE8B}">
+  <dimension ref="A1:AAA16"/>
+  <sheetViews>
+    <sheetView zoomScale="119" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="88.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="HA3" s="4"/>
+      <c r="AAA3" s="5"/>
+    </row>
+    <row r="4" spans="1:703">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703">
+      <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:703">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:703">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:703">
+      <c r="A11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:703">
+      <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:703">
+      <c r="A13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:703">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:703">
+      <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:703">
+      <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="beginsWith" dxfId="88" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="87" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="86" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="expression" dxfId="85" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="84" priority="10">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14DC7B17-F493-C84F-A382-5EE6E86AC515}">
+  <dimension ref="A1:AAA27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="71.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703">
+      <c r="A1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703">
+      <c r="A2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703">
+      <c r="A3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
+    </row>
+    <row r="4" spans="1:703">
+      <c r="A4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="HA4" s="6"/>
+      <c r="AAA4" s="6"/>
+    </row>
+    <row r="5" spans="1:703">
+      <c r="A5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="HA5" s="6"/>
+      <c r="AAA5" s="6"/>
+    </row>
+    <row r="6" spans="1:703">
+      <c r="A6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703">
+      <c r="A7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703">
+      <c r="A8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703">
+      <c r="A9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+    <row r="10" spans="1:703">
+      <c r="A10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="HA10" s="4"/>
+      <c r="AAA10" s="5"/>
+    </row>
+    <row r="11" spans="1:703">
+      <c r="A11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="HA11" s="4"/>
+      <c r="AAA11" s="5"/>
+    </row>
+    <row r="12" spans="1:703">
+      <c r="A12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="HA12" s="4"/>
+      <c r="AAA12" s="5"/>
+    </row>
+    <row r="13" spans="1:703">
+      <c r="A13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:703">
+      <c r="A14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:703">
+      <c r="A15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:703">
+      <c r="A16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="54">
+      <c r="A21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="54">
+      <c r="A23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="36">
+      <c r="A24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="36">
+      <c r="A25" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="36">
+      <c r="A26" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="54">
+      <c r="A27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <sortState ref="A4:B18">
+    <sortCondition ref="A4:A18"/>
+  </sortState>
+  <conditionalFormatting sqref="A20:A22 A4:A15 A24 A28:A1048576">
+    <cfRule type="beginsWith" dxfId="83" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A4,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="82" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A4,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="81" priority="42" stopIfTrue="1">
+      <formula>LEN(TRIM(A4))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B10 B20:B22 B12:B15 B24 B28:B1048576">
+    <cfRule type="expression" dxfId="80" priority="43" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="79" priority="44">
+      <formula>LEN(TRIM(B4))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="beginsWith" dxfId="78" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="77" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="76" priority="34" stopIfTrue="1">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="beginsWith" dxfId="75" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A17,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="74" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A17,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="73" priority="31" stopIfTrue="1">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18:A19">
+    <cfRule type="beginsWith" dxfId="72" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A18,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="71" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A18,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="70" priority="28" stopIfTrue="1">
+      <formula>LEN(TRIM(A18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A3">
+    <cfRule type="beginsWith" dxfId="69" priority="21" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="68" priority="22" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="67" priority="23" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B3">
+    <cfRule type="expression" dxfId="66" priority="24" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="65" priority="25">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="beginsWith" dxfId="64" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="63" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="62" priority="18" stopIfTrue="1">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23">
+    <cfRule type="expression" dxfId="61" priority="19" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="60" priority="20">
+      <formula>LEN(TRIM(B23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="beginsWith" dxfId="59" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="58" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="57" priority="13" stopIfTrue="1">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25">
+    <cfRule type="expression" dxfId="56" priority="14" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="55" priority="15">
+      <formula>LEN(TRIM(B25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="beginsWith" dxfId="54" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="53" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="52" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="expression" dxfId="51" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="50" priority="10">
+      <formula>LEN(TRIM(B27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="beginsWith" dxfId="49" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A26,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="48" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A26,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="47" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26">
+    <cfRule type="expression" dxfId="46" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="45" priority="5">
+      <formula>LEN(TRIM(B26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17A18B9-A7F4-B848-8E0C-853951D12261}">
+  <dimension ref="A1:AAA9"/>
+  <sheetViews>
+    <sheetView zoomScale="118" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection sqref="A1:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="23.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="209:703">
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="209:703">
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="209:703">
+      <c r="HA3" s="4"/>
+      <c r="AAA3" s="5"/>
+    </row>
+    <row r="4" spans="209:703">
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="209:703">
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="209:703">
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="209:703">
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="209:703">
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="209:703">
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A13:A1048576">
+    <cfRule type="beginsWith" dxfId="44" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="43" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="42" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:B1048576">
+    <cfRule type="expression" dxfId="41" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="40" priority="10">
+      <formula>LEN(TRIM(B13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A12">
+    <cfRule type="beginsWith" dxfId="39" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="38" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="37" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B12">
+    <cfRule type="expression" dxfId="36" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="35" priority="5">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37D3F2F-6FA3-E945-A3ED-EFC8DABE8040}">
+  <dimension ref="A1:AAA10"/>
+  <sheetViews>
+    <sheetView zoomScale="118" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -887,153 +3257,355 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="HA3" s="4"/>
       <c r="AAA3" s="5"/>
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>56</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:703">
-      <c r="A11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:703">
-      <c r="A12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:703">
-      <c r="A13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="6" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A13:A1048576">
+    <cfRule type="beginsWith" dxfId="34" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="33" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="32" priority="13" stopIfTrue="1">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:B1048576">
+    <cfRule type="expression" dxfId="31" priority="14" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="30" priority="15">
+      <formula>LEN(TRIM(B13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:A12">
+    <cfRule type="beginsWith" dxfId="29" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A11,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="28" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A11,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="27" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:B12">
+    <cfRule type="expression" dxfId="26" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="25" priority="10">
+      <formula>LEN(TRIM(B11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A10">
+    <cfRule type="beginsWith" dxfId="24" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="5" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="23" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B4 B9:B1048576">
-    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B10">
+    <cfRule type="expression" dxfId="21" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B8">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938A5DF5-858F-F04F-A650-D78F3893CC59}">
+  <dimension ref="A1:AAA9"/>
+  <sheetViews>
+    <sheetView zoomScale="118" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection sqref="A1:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="23.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="209:703">
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="209:703">
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="209:703">
+      <c r="HA3" s="4"/>
+      <c r="AAA3" s="5"/>
+    </row>
+    <row r="4" spans="209:703">
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="209:703">
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="209:703">
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="209:703">
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="209:703">
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="209:703">
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A13:A1048576">
+    <cfRule type="beginsWith" dxfId="19" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="18" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="17" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:B1048576">
+    <cfRule type="expression" dxfId="16" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
-      <formula>LEN(TRIM(B5))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="15" priority="10">
+      <formula>LEN(TRIM(B13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A12">
+    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="13" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="12" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B12">
+    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="10" priority="5">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4394A7E7-FE1D-A34C-9EEB-381E60F2B1B4}">
+  <dimension ref="A1:AAA9"/>
+  <sheetViews>
+    <sheetView zoomScale="118" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection sqref="A1:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="23.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="209:703">
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="209:703">
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="209:703">
+      <c r="HA3" s="4"/>
+      <c r="AAA3" s="5"/>
+    </row>
+    <row r="4" spans="209:703">
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="209:703">
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="209:703">
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="209:703">
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="209:703">
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="209:703">
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A13:A1048576">
+    <cfRule type="beginsWith" dxfId="9" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="8" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:B1048576">
+    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="10">
+      <formula>LEN(TRIM(B13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A12">
+    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B12">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added documentation for `saveTableAsCsv`
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-03.data.xlsx
+++ b/artifact/data/web-03.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0F0D3B-68C9-C94B-95D0-34D1F8473B03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BD6FF2-C506-7F4E-AC80-A08A366521C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="10500" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="10500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="195">
   <si>
     <t>true</t>
   </si>
@@ -572,6 +572,81 @@
   </si>
   <si>
     <t>${aut.example2.loc}//thead//th[text()='Office']</t>
+  </si>
+  <si>
+    <t>aut.example3.url</t>
+  </si>
+  <si>
+    <t>aut.example3.content.expected</t>
+  </si>
+  <si>
+    <t>aut.example3.content.loc</t>
+  </si>
+  <si>
+    <t>aut.example3.heading.loc</t>
+  </si>
+  <si>
+    <t>aut.example3.content.saveTo</t>
+  </si>
+  <si>
+    <t>aut.example3.heading.text</t>
+  </si>
+  <si>
+    <t>aut.example3.loc</t>
+  </si>
+  <si>
+    <t>aut.example3.next.loc</t>
+  </si>
+  <si>
+    <t>https://material.angular.io/components/table/overview</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/web-03-example3.csv</t>
+  </si>
+  <si>
+    <t>xpath=${aut.example3.loc}//tbody//td</t>
+  </si>
+  <si>
+    <t>$(syspath|out|fullpath)/example3.csv</t>
+  </si>
+  <si>
+    <t>${aut.example3.loc}//thead//th</t>
+  </si>
+  <si>
+    <t>${aut.example3.loc}//thead//th[text()='Symbol']</t>
+  </si>
+  <si>
+    <t>No.,Name,Weight,Symbol</t>
+  </si>
+  <si>
+    <t>//button[contains(@class,'mat-paginator-navigation-next')]</t>
+  </si>
+  <si>
+    <t>aut.example3.heading.Symbol.loc</t>
+  </si>
+  <si>
+    <t>//div[@material-docs-example="table-pagination"]//table[contains(@class,'mat-table')]</t>
+  </si>
+  <si>
+    <t>//h4[ contains(text(),'Pagination') ]/following-sibling::div//table[ contains(@class,'mat-table') ]</t>
+  </si>
+  <si>
+    <t>example1.url</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?q=Nexial</t>
+  </si>
+  <si>
+    <t>example1.target.text</t>
+  </si>
+  <si>
+    <t>example1.target.url</t>
+  </si>
+  <si>
+    <t>https://nexiality.github.io/documentation/userguide/HistoryOfNexial</t>
+  </si>
+  <si>
+    <t>link=History of Nexial | Nexial Automation</t>
   </si>
 </sst>
 </file>
@@ -2463,7 +2538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -3792,15 +3867,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938A5DF5-858F-F04F-A650-D78F3893CC59}">
-  <dimension ref="A1:AAA16"/>
+  <dimension ref="A1:AAA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A10" zoomScale="114" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="69.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
@@ -3953,6 +4028,81 @@
       </c>
       <c r="B16" s="2" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -4019,7 +4169,7 @@
   <dimension ref="A1:AAA9"/>
   <sheetViews>
     <sheetView zoomScale="118" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection sqref="A1:C13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -4031,39 +4181,57 @@
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="209:703">
+    <row r="1" spans="1:703">
+      <c r="A1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
-    <row r="2" spans="209:703">
+    <row r="2" spans="1:703">
+      <c r="A2" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>194</v>
+      </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
-    <row r="3" spans="209:703">
+    <row r="3" spans="1:703">
+      <c r="A3" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="HA3" s="4"/>
       <c r="AAA3" s="5"/>
     </row>
-    <row r="4" spans="209:703">
+    <row r="4" spans="1:703">
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
-    <row r="5" spans="209:703">
+    <row r="5" spans="1:703">
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
-    <row r="6" spans="209:703">
+    <row r="6" spans="1:703">
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
-    <row r="7" spans="209:703">
+    <row r="7" spans="1:703">
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
-    <row r="8" spans="209:703">
+    <row r="8" spans="1:703">
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
-    <row r="9" spans="209:703">
+    <row r="9" spans="1:703">
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>

</xml_diff>

<commit_message>
massive changes to get ready for proper tutorial site. now ready for local jekyll rendering as well.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-03.data.xlsx
+++ b/artifact/data/web-03.data.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BD6FF2-C506-7F4E-AC80-A08A366521C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427B5EDA-D6F3-514F-AB57-8DB763B4F610}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="10500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
     <sheet name="locators-class" sheetId="3" r:id="rId2"/>
-    <sheet name="locators-css" sheetId="4" r:id="rId3"/>
-    <sheet name="locators-id" sheetId="5" r:id="rId4"/>
-    <sheet name="locators-tag" sheetId="6" r:id="rId5"/>
+    <sheet name="locators-link" sheetId="9" r:id="rId3"/>
+    <sheet name="locators-tag" sheetId="6" r:id="rId4"/>
+    <sheet name="locators-id" sheetId="5" r:id="rId5"/>
     <sheet name="locators-name" sheetId="7" r:id="rId6"/>
-    <sheet name="locators-xpath" sheetId="8" r:id="rId7"/>
-    <sheet name="locators-link" sheetId="9" r:id="rId8"/>
+    <sheet name="locators-css" sheetId="4" r:id="rId7"/>
+    <sheet name="locators-xpath" sheetId="8" r:id="rId8"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId9"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="192">
   <si>
     <t>true</t>
   </si>
@@ -333,12 +333,6 @@
     <t>id=heading</t>
   </si>
   <si>
-    <t>nexial.highlight</t>
-  </si>
-  <si>
-    <t>nexial.highlightWaitMs</t>
-  </si>
-  <si>
     <t>aut : error : tc2</t>
   </si>
   <si>
@@ -362,9 +356,6 @@
   <si>
     <t>Please fill in Message
 X</t>
-  </si>
-  <si>
-    <t>500</t>
   </si>
   <si>
     <t>nexial.browser.forceJSClick</t>
@@ -789,7 +780,44 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="113">
+  <dxfs count="103">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -922,43 +950,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1024,6 +1015,43 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1089,43 +1117,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1321,43 +1312,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1553,6 +1507,117 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1618,6 +1683,43 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1641,247 +1743,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2538,7 +2399,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -2690,40 +2553,40 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1 A3:A9 A22:A1048576">
-    <cfRule type="beginsWith" dxfId="112" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="102" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="111" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="101" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="110" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="100" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1 B3:B9 B22:B1048576">
-    <cfRule type="expression" dxfId="109" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="108" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="98" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="beginsWith" dxfId="107" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="97" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="106" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="96" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="105" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="95" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="104" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="103" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="93" priority="5">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2740,7 +2603,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="88.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
@@ -2841,21 +2704,21 @@
     <sortCondition ref="A1:A9"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="102" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="92" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="101" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="91" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="100" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="90" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="99" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="98" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="88" priority="12">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2865,15 +2728,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CC5913-9CC1-104B-A93C-2AE9134DFE8B}">
-  <dimension ref="A1:AAA16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4394A7E7-FE1D-A34C-9EEB-381E60F2B1B4}">
+  <dimension ref="A1:AAA9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="88.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.1640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="81.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
@@ -2881,164 +2744,95 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>186</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>187</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>188</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>191</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>189</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>190</v>
       </c>
       <c r="HA3" s="4"/>
       <c r="AAA3" s="5"/>
     </row>
     <row r="4" spans="1:703">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
-      <c r="A6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
-      <c r="A8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
     </row>
     <row r="9" spans="1:703">
-      <c r="A9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:703">
-      <c r="A10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:703">
-      <c r="A11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:703">
-      <c r="A12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:703">
-      <c r="A13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:703">
-      <c r="A14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:703">
-      <c r="A15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:703">
-      <c r="A16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="97" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+  <conditionalFormatting sqref="A13:A1048576">
+    <cfRule type="beginsWith" dxfId="87" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="86" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="85" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:B1048576">
+    <cfRule type="expression" dxfId="84" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="83" priority="10">
+      <formula>LEN(TRIM(B13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A12">
+    <cfRule type="beginsWith" dxfId="82" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="96" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="81" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="95" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="94" priority="9" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B12">
+    <cfRule type="expression" dxfId="79" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="93" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3048,429 +2842,15 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14DC7B17-F493-C84F-A382-5EE6E86AC515}">
-  <dimension ref="A1:AAA27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17A18B9-A7F4-B848-8E0C-853951D12261}">
+  <dimension ref="A1:AAA8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="71.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:703">
-      <c r="A1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="HA1" s="6"/>
-      <c r="AAA1" s="6"/>
-    </row>
-    <row r="2" spans="1:703">
-      <c r="A2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="HA2" s="6"/>
-      <c r="AAA2" s="6"/>
-    </row>
-    <row r="3" spans="1:703">
-      <c r="A3" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="HA3" s="6"/>
-      <c r="AAA3" s="6"/>
-    </row>
-    <row r="4" spans="1:703">
-      <c r="A4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="HA4" s="6"/>
-      <c r="AAA4" s="6"/>
-    </row>
-    <row r="5" spans="1:703">
-      <c r="A5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="HA5" s="6"/>
-      <c r="AAA5" s="6"/>
-    </row>
-    <row r="6" spans="1:703">
-      <c r="A6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="HA6" s="4"/>
-      <c r="AAA6" s="5"/>
-    </row>
-    <row r="7" spans="1:703">
-      <c r="A7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="HA7" s="4"/>
-      <c r="AAA7" s="5"/>
-    </row>
-    <row r="8" spans="1:703">
-      <c r="A8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="HA8" s="4"/>
-      <c r="AAA8" s="5"/>
-    </row>
-    <row r="9" spans="1:703">
-      <c r="A9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="HA9" s="4"/>
-      <c r="AAA9" s="5"/>
-    </row>
-    <row r="10" spans="1:703">
-      <c r="A10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="HA10" s="4"/>
-      <c r="AAA10" s="5"/>
-    </row>
-    <row r="11" spans="1:703">
-      <c r="A11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="HA11" s="4"/>
-      <c r="AAA11" s="5"/>
-    </row>
-    <row r="12" spans="1:703">
-      <c r="A12" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="HA12" s="4"/>
-      <c r="AAA12" s="5"/>
-    </row>
-    <row r="13" spans="1:703">
-      <c r="A13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:703">
-      <c r="A14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:703">
-      <c r="A15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:703">
-      <c r="A16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="54">
-      <c r="A21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="54">
-      <c r="A23" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="36">
-      <c r="A24" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="36">
-      <c r="A25" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="36">
-      <c r="A26" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="54">
-      <c r="A27" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <sortState ref="A4:B18">
-    <sortCondition ref="A4:A18"/>
-  </sortState>
-  <conditionalFormatting sqref="A20:A22 A4:A15 A24 A28:A1048576">
-    <cfRule type="beginsWith" dxfId="92" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A4,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="91" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A4,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="90" priority="42" stopIfTrue="1">
-      <formula>LEN(TRIM(A4))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:B10 B20:B22 B12:B15 B24 B28:B1048576">
-    <cfRule type="expression" dxfId="89" priority="43" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="88" priority="44">
-      <formula>LEN(TRIM(B4))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="beginsWith" dxfId="87" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="86" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="85" priority="34" stopIfTrue="1">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="beginsWith" dxfId="84" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A17,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="83" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A17,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="82" priority="31" stopIfTrue="1">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18:A19">
-    <cfRule type="beginsWith" dxfId="81" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A18,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="80" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A18,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="79" priority="28" stopIfTrue="1">
-      <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A3">
-    <cfRule type="beginsWith" dxfId="78" priority="21" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="77" priority="22" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="76" priority="23" stopIfTrue="1">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B3">
-    <cfRule type="expression" dxfId="75" priority="24" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="74" priority="25">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="beginsWith" dxfId="73" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="72" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="71" priority="18" stopIfTrue="1">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="70" priority="19" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="69" priority="20">
-      <formula>LEN(TRIM(B23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="beginsWith" dxfId="68" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="67" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="66" priority="13" stopIfTrue="1">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="65" priority="14" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="64" priority="15">
-      <formula>LEN(TRIM(B25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="beginsWith" dxfId="63" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="62" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="61" priority="8" stopIfTrue="1">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="60" priority="9" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="59" priority="10">
-      <formula>LEN(TRIM(B27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="beginsWith" dxfId="58" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A26,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="57" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A26,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="56" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26">
-    <cfRule type="expression" dxfId="55" priority="4" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="54" priority="5">
-      <formula>LEN(TRIM(B26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17A18B9-A7F4-B848-8E0C-853951D12261}">
-  <dimension ref="A1:AAA10"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
-  <cols>
-    <col min="1" max="1" width="23.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="51.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
@@ -3481,68 +2861,56 @@
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="HA2" s="6"/>
-      <c r="AAA2" s="6"/>
+        <v>127</v>
+      </c>
+      <c r="HA2" s="4"/>
+      <c r="AAA2" s="5"/>
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="HA3" s="6"/>
-      <c r="AAA3" s="6"/>
+        <v>129</v>
+      </c>
+      <c r="HA3" s="4"/>
+      <c r="AAA3" s="5"/>
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>130</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
-      <c r="A6" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703">
-      <c r="A7" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
@@ -3550,63 +2918,409 @@
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
-    <row r="9" spans="1:703">
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A2:A1048576">
+    <cfRule type="beginsWith" dxfId="77" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="76" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="75" priority="11" stopIfTrue="1">
+      <formula>LEN(TRIM(A2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="expression" dxfId="74" priority="12" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="73" priority="13">
+      <formula>LEN(TRIM(B2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="beginsWith" dxfId="72" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="71" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="70" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14DC7B17-F493-C84F-A382-5EE6E86AC515}">
+  <dimension ref="A1:AAA25"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="71.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703" ht="19" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703" ht="19" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703" ht="19" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
+    </row>
+    <row r="4" spans="1:703" ht="19" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703" ht="19" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703" ht="19" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703" ht="19" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703" ht="19" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703" ht="19" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
-    <row r="10" spans="1:703">
+    <row r="10" spans="1:703" ht="19" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="HA10" s="4"/>
       <c r="AAA10" s="5"/>
     </row>
+    <row r="11" spans="1:703" ht="19" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:703" ht="19" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:703" ht="19" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:703" ht="19" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:703" ht="19" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:703" ht="19" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="19" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="19" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="54">
+      <c r="A20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="36">
+      <c r="A21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="36">
+      <c r="A22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="36">
+      <c r="A23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="54">
+      <c r="A25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A14:A1048576">
-    <cfRule type="beginsWith" dxfId="53" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+  <sortState ref="A17:B25">
+    <sortCondition ref="A17:A25"/>
+  </sortState>
+  <conditionalFormatting sqref="A18:A20 A22 A26:A1048576 A1:A13">
+    <cfRule type="beginsWith" dxfId="69" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="68" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="67" priority="42" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:B20 B10:B13 B22 B26:B1048576 B1:B8">
+    <cfRule type="expression" dxfId="66" priority="43" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="65" priority="44">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="beginsWith" dxfId="64" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="52" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="63" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="51" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="34" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:B1048576">
-    <cfRule type="expression" dxfId="50" priority="12" stopIfTrue="1">
+  <conditionalFormatting sqref="A15">
+    <cfRule type="beginsWith" dxfId="61" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="60" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="59" priority="31" stopIfTrue="1">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16:A17">
+    <cfRule type="beginsWith" dxfId="58" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="57" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="56" priority="28" stopIfTrue="1">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="beginsWith" dxfId="55" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A21,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="54" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A21,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="53" priority="18" stopIfTrue="1">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="expression" dxfId="52" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="49" priority="13">
-      <formula>LEN(TRIM(B14))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="51" priority="20">
+      <formula>LEN(TRIM(B21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A13">
-    <cfRule type="beginsWith" dxfId="48" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="47" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="46" priority="6" stopIfTrue="1">
-      <formula>LEN(TRIM(A2))&gt;0</formula>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="beginsWith" dxfId="50" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="49" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="48" priority="13" stopIfTrue="1">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B13">
-    <cfRule type="expression" dxfId="45" priority="7" stopIfTrue="1">
+  <conditionalFormatting sqref="B23">
+    <cfRule type="expression" dxfId="47" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="44" priority="8">
-      <formula>LEN(TRIM(B2))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="46" priority="15">
+      <formula>LEN(TRIM(B23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="beginsWith" dxfId="43" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="42" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="41" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="beginsWith" dxfId="45" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="44" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="43" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25">
+    <cfRule type="expression" dxfId="42" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="41" priority="10">
+      <formula>LEN(TRIM(B25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="beginsWith" dxfId="40" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A24,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="39" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A24,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="38" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="expression" dxfId="37" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="36" priority="5">
+      <formula>LEN(TRIM(B24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3616,14 +3330,446 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37D3F2F-6FA3-E945-A3ED-EFC8DABE8040}">
-  <dimension ref="A1:AAA17"/>
+  <dimension ref="A1:AAA22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.1640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.83203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="80.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703" ht="19" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703" ht="19" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703" ht="19" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="HA3" s="4"/>
+      <c r="AAA3" s="5"/>
+    </row>
+    <row r="4" spans="1:703" ht="19" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703" ht="19" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703" ht="19" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703" ht="19" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703" ht="19" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703" ht="19" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+    <row r="10" spans="1:703" ht="19" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:703" ht="19" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:703" ht="19" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:703" ht="19" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:703" ht="19" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:703" ht="19" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:703" ht="19" customHeight="1"/>
+    <row r="17" ht="19" customHeight="1"/>
+    <row r="18" ht="19" customHeight="1"/>
+    <row r="19" ht="19" customHeight="1"/>
+    <row r="20" ht="19" customHeight="1"/>
+    <row r="21" ht="19" customHeight="1"/>
+    <row r="22" ht="19" customHeight="1"/>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <sortState ref="A1:B15">
+    <sortCondition ref="A1:A15"/>
+  </sortState>
+  <conditionalFormatting sqref="A13:A1048576">
+    <cfRule type="beginsWith" dxfId="35" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="34" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="33" priority="16" stopIfTrue="1">
+      <formula>LEN(TRIM(A13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:B1048576">
+    <cfRule type="expression" dxfId="32" priority="17" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="31" priority="18">
+      <formula>LEN(TRIM(B13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:A12">
+    <cfRule type="beginsWith" dxfId="30" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A11,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="29" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A11,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="28" priority="11" stopIfTrue="1">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:B12">
+    <cfRule type="expression" dxfId="27" priority="12" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="26" priority="13">
+      <formula>LEN(TRIM(B11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A10">
+    <cfRule type="beginsWith" dxfId="25" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="24" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="23" priority="6" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B10">
+    <cfRule type="expression" dxfId="22" priority="7" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="21" priority="8">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CC5913-9CC1-104B-A93C-2AE9134DFE8B}">
+  <dimension ref="A1:AAA35"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="24" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="88.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703" ht="19" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703" ht="19" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703" ht="19" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="HA3" s="4"/>
+      <c r="AAA3" s="5"/>
+    </row>
+    <row r="4" spans="1:703" ht="19" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703" ht="19" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703" ht="19" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703" ht="19" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703" ht="19" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:703" ht="19" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:703" ht="19" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:703" ht="19" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:703" ht="19" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:703" ht="19" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:703" ht="19" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:703" ht="19" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:703" ht="19" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" ht="19" customHeight="1"/>
+    <row r="18" ht="19" customHeight="1"/>
+    <row r="19" ht="19" customHeight="1"/>
+    <row r="20" ht="19" customHeight="1"/>
+    <row r="21" ht="19" customHeight="1"/>
+    <row r="22" ht="19" customHeight="1"/>
+    <row r="23" ht="19" customHeight="1"/>
+    <row r="24" ht="19" customHeight="1"/>
+    <row r="25" ht="19" customHeight="1"/>
+    <row r="26" ht="19" customHeight="1"/>
+    <row r="27" ht="19" customHeight="1"/>
+    <row r="28" ht="19" customHeight="1"/>
+    <row r="29" ht="19" customHeight="1"/>
+    <row r="30" ht="19" customHeight="1"/>
+    <row r="31" ht="19" customHeight="1"/>
+    <row r="32" ht="19" customHeight="1"/>
+    <row r="33" ht="19" customHeight="1"/>
+    <row r="34" ht="19" customHeight="1"/>
+    <row r="35" ht="19" customHeight="1"/>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <sortState ref="A1:B16">
+    <sortCondition ref="A1:A16"/>
+  </sortState>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="beginsWith" dxfId="17" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="16" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="15" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="expression" dxfId="14" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="13" priority="10">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938A5DF5-858F-F04F-A650-D78F3893CC59}">
+  <dimension ref="A1:AAA25"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="103.1640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
@@ -3631,648 +3777,279 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>142</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>154</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
-    <row r="3" spans="1:703" ht="23" customHeight="1">
+    <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>151</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
-    <row r="4" spans="1:703" ht="23" customHeight="1">
+    <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="HA4" s="6"/>
-      <c r="AAA4" s="6"/>
-    </row>
-    <row r="5" spans="1:703" ht="23" customHeight="1">
+        <v>155</v>
+      </c>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
-    <row r="6" spans="1:703" ht="23" customHeight="1">
+    <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>115</v>
+        <v>152</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
-    <row r="7" spans="1:703" ht="23" customHeight="1">
+    <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
-    <row r="8" spans="1:703" ht="23" customHeight="1">
+    <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
-    <row r="9" spans="1:703" ht="23" customHeight="1">
+    <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>110</v>
+        <v>157</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
-    <row r="10" spans="1:703" ht="23" customHeight="1">
+    <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
-        <v>123</v>
+        <v>163</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="HA10" s="4"/>
       <c r="AAA10" s="5"/>
     </row>
-    <row r="11" spans="1:703" ht="23" customHeight="1">
+    <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
-        <v>106</v>
+        <v>144</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="HA11" s="4"/>
-      <c r="AAA11" s="5"/>
-    </row>
-    <row r="12" spans="1:703" ht="23" customHeight="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:703">
       <c r="A12" s="1" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:703" ht="23" customHeight="1">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:703">
       <c r="A13" s="1" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:703" ht="23" customHeight="1">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:703">
       <c r="A14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:703" ht="23" customHeight="1">
+        <v>156</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:703">
       <c r="A15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:703" ht="27" customHeight="1">
+        <v>161</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:703">
       <c r="A16" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="23" customHeight="1">
+        <v>147</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>113</v>
+        <v>168</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <sortState ref="A4:B17">
-    <sortCondition ref="A4:A17"/>
+  <sortState ref="A1:B25">
+    <sortCondition ref="A1:A25"/>
   </sortState>
   <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="beginsWith" dxfId="40" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="12" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="39" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="11" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="38" priority="16" stopIfTrue="1">
-      <formula>LEN(TRIM(A15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:B1048576">
-    <cfRule type="expression" dxfId="37" priority="17" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="36" priority="18">
-      <formula>LEN(TRIM(B15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:A14">
-    <cfRule type="beginsWith" dxfId="35" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="34" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="33" priority="11" stopIfTrue="1">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:B14">
-    <cfRule type="expression" dxfId="32" priority="12" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="31" priority="13">
-      <formula>LEN(TRIM(B13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A12">
-    <cfRule type="beginsWith" dxfId="30" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A3,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="29" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A3,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="28" priority="6" stopIfTrue="1">
-      <formula>LEN(TRIM(A3))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B12">
-    <cfRule type="expression" dxfId="27" priority="7" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="26" priority="8">
-      <formula>LEN(TRIM(B3))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A2">
-    <cfRule type="beginsWith" dxfId="25" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="23" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938A5DF5-858F-F04F-A650-D78F3893CC59}">
-  <dimension ref="A1:AAA25"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="114" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
-  <cols>
-    <col min="1" max="1" width="30.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="69.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:703">
-      <c r="A1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="HA1" s="6"/>
-      <c r="AAA1" s="6"/>
-    </row>
-    <row r="2" spans="1:703">
-      <c r="A2" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="HA2" s="6"/>
-      <c r="AAA2" s="6"/>
-    </row>
-    <row r="3" spans="1:703">
-      <c r="A3" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="HA3" s="6"/>
-      <c r="AAA3" s="6"/>
-    </row>
-    <row r="4" spans="1:703">
-      <c r="A4" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="HA4" s="4"/>
-      <c r="AAA4" s="5"/>
-    </row>
-    <row r="5" spans="1:703">
-      <c r="A5" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="HA5" s="4"/>
-      <c r="AAA5" s="5"/>
-    </row>
-    <row r="6" spans="1:703">
-      <c r="A6" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="HA6" s="4"/>
-      <c r="AAA6" s="5"/>
-    </row>
-    <row r="7" spans="1:703">
-      <c r="A7" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="HA7" s="4"/>
-      <c r="AAA7" s="5"/>
-    </row>
-    <row r="8" spans="1:703">
-      <c r="A8" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="HA8" s="4"/>
-      <c r="AAA8" s="5"/>
-    </row>
-    <row r="9" spans="1:703">
-      <c r="A9" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="HA9" s="4"/>
-      <c r="AAA9" s="5"/>
-    </row>
-    <row r="10" spans="1:703">
-      <c r="A10" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="HA10" s="4"/>
-      <c r="AAA10" s="5"/>
-    </row>
-    <row r="11" spans="1:703">
-      <c r="A11" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:703">
-      <c r="A12" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="13" spans="1:703">
-      <c r="A13" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:703">
-      <c r="A14" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="15" spans="1:703">
-      <c r="A15" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:703">
-      <c r="A16" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <sortState ref="A1:B16">
-    <sortCondition ref="A1:A16"/>
-  </sortState>
-  <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="beginsWith" dxfId="22" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="21" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="20" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B1048576 B13:B14">
-    <cfRule type="expression" dxfId="19" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="13">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="beginsWith" dxfId="17" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="7" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="6" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="15" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B13">
-    <cfRule type="expression" dxfId="14" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="13" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="12" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="11" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4394A7E7-FE1D-A34C-9EEB-381E60F2B1B4}">
-  <dimension ref="A1:AAA9"/>
-  <sheetViews>
-    <sheetView zoomScale="118" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
-  <cols>
-    <col min="1" max="1" width="23.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.6640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:703">
-      <c r="A1" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="HA1" s="6"/>
-      <c r="AAA1" s="6"/>
-    </row>
-    <row r="2" spans="1:703">
-      <c r="A2" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="HA2" s="6"/>
-      <c r="AAA2" s="6"/>
-    </row>
-    <row r="3" spans="1:703">
-      <c r="A3" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="HA3" s="4"/>
-      <c r="AAA3" s="5"/>
-    </row>
-    <row r="4" spans="1:703">
-      <c r="HA4" s="4"/>
-      <c r="AAA4" s="5"/>
-    </row>
-    <row r="5" spans="1:703">
-      <c r="HA5" s="4"/>
-      <c r="AAA5" s="5"/>
-    </row>
-    <row r="6" spans="1:703">
-      <c r="HA6" s="4"/>
-      <c r="AAA6" s="5"/>
-    </row>
-    <row r="7" spans="1:703">
-      <c r="HA7" s="4"/>
-      <c r="AAA7" s="5"/>
-    </row>
-    <row r="8" spans="1:703">
-      <c r="HA8" s="4"/>
-      <c r="AAA8" s="5"/>
-    </row>
-    <row r="9" spans="1:703">
-      <c r="HA9" s="4"/>
-      <c r="AAA9" s="5"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="9" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
-      <formula>LEN(TRIM(A13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="10">
-      <formula>LEN(TRIM(B13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A12">
-    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B12">
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- [`nexial.web.unfocusAfterType`](../systemvars/index#nexial.web.unfocusAfterType): support automation to blur the   target web element after entering input. - change default of `nexial.web.preemptiveAlertCheck` to `false` (was `true`). Modern web app seldom uses JS alert anymore. - reworked system variable documentation; fixed typos.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-03.data.xlsx
+++ b/artifact/data/web-03.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427B5EDA-D6F3-514F-AB57-8DB763B4F610}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4375CCD1-33C6-174A-A6EF-ED881E4003E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="6840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="195">
   <si>
     <t>true</t>
   </si>
@@ -91,9 +91,6 @@
     <t>https://en.wikipedia.org/wiki/%22Hello,_World!%22_program</t>
   </si>
   <si>
-    <t>750</t>
-  </si>
-  <si>
     <t>250</t>
   </si>
   <si>
@@ -101,12 +98,6 @@
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>//nexial.highlightWaitMs</t>
-  </si>
-  <si>
-    <t>//nexial.highlight</t>
   </si>
   <si>
     <t>aut : tocTitle</t>
@@ -637,7 +628,25 @@
     <t>https://nexiality.github.io/documentation/userguide/HistoryOfNexial</t>
   </si>
   <si>
-    <t>link=History of Nexial | Nexial Automation</t>
+    <t>example1.target.product</t>
+  </si>
+  <si>
+    <t>Nexial</t>
+  </si>
+  <si>
+    <t>link=History of ${example1.target.product} | ${example1.target.product} Automation</t>
+  </si>
+  <si>
+    <t>nexial.web.unfocusAfterType</t>
+  </si>
+  <si>
+    <t>nexial.highlight</t>
+  </si>
+  <si>
+    <t>nexial.highlightWaitMs</t>
+  </si>
+  <si>
+    <t>500</t>
   </si>
 </sst>
 </file>
@@ -780,7 +789,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="103">
+  <dxfs count="100">
     <dxf>
       <font>
         <b/>
@@ -973,43 +982,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2399,9 +2371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -2424,10 +2394,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
@@ -2437,7 +2407,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
@@ -2484,7 +2454,7 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>192</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
@@ -2494,10 +2464,10 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>193</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>194</v>
       </c>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
@@ -2553,40 +2523,40 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1 A3:A9 A22:A1048576">
-    <cfRule type="beginsWith" dxfId="102" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="99" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="101" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="98" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="100" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="97" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1 B3:B9 B22:B1048576">
-    <cfRule type="expression" dxfId="99" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="98" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="95" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="beginsWith" dxfId="97" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="94" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="96" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="93" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="95" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="92" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="94" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="93" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="90" priority="5">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2612,50 +2582,50 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="HA3" s="4"/>
       <c r="AAA3" s="5"/>
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
@@ -2672,30 +2642,30 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2704,21 +2674,21 @@
     <sortCondition ref="A1:A9"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="92" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="89" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="91" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="88" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="90" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="87" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="89" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="88" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="85" priority="12">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2731,11 +2701,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4394A7E7-FE1D-A34C-9EEB-381E60F2B1B4}">
   <dimension ref="A1:AAA9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScale="123" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="81.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
@@ -2744,35 +2714,41 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="HA3" s="4"/>
       <c r="AAA3" s="5"/>
     </row>
     <row r="4" spans="1:703">
+      <c r="A4" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
@@ -2799,40 +2775,40 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="87" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="84" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="86" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="83" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="85" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="84" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="83" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A12">
-    <cfRule type="beginsWith" dxfId="82" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="79" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="81" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="78" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="80" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B12">
-    <cfRule type="expression" dxfId="79" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="78" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2861,7 +2837,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
@@ -2871,37 +2847,37 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="HA2" s="4"/>
       <c r="AAA2" s="5"/>
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="HA3" s="4"/>
       <c r="AAA3" s="5"/>
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
@@ -2921,32 +2897,32 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="beginsWith" dxfId="77" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="74" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="76" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="73" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="75" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="74" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="73" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="13">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="beginsWith" dxfId="72" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="69" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="71" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="68" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="70" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2959,7 +2935,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14DC7B17-F493-C84F-A382-5EE6E86AC515}">
   <dimension ref="A1:AAA25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView topLeftCell="A18" zoomScale="107" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -2972,7 +2950,7 @@
   <sheetData>
     <row r="1" spans="1:703" ht="19" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -2982,132 +2960,132 @@
     </row>
     <row r="2" spans="1:703" ht="19" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703" ht="19" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
     <row r="4" spans="1:703" ht="19" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703" ht="19" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703" ht="19" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703" ht="19" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703" ht="19" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
     <row r="9" spans="1:703" ht="19" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
     <row r="10" spans="1:703" ht="19" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="HA10" s="4"/>
       <c r="AAA10" s="5"/>
     </row>
     <row r="11" spans="1:703" ht="19" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:703" ht="19" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:703" ht="19" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:703" ht="19" customHeight="1">
       <c r="A14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:703" ht="19" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:703" ht="19" customHeight="1">
@@ -3115,79 +3093,79 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19" customHeight="1">
       <c r="A18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="54">
       <c r="A20" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="36">
       <c r="A21" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="36">
       <c r="A22" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="36">
       <c r="A23" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="54">
       <c r="A25" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -3196,130 +3174,130 @@
     <sortCondition ref="A17:A25"/>
   </sortState>
   <conditionalFormatting sqref="A18:A20 A22 A26:A1048576 A1:A13">
-    <cfRule type="beginsWith" dxfId="69" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="66" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="68" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="65" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="67" priority="42" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="42" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 B10:B13 B22 B26:B1048576 B1:B8">
-    <cfRule type="expression" dxfId="66" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="43" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="65" priority="44">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="44">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="64" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="61" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="63" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="60" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="62" priority="34" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="34" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="beginsWith" dxfId="61" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="58" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="60" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="57" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="59" priority="31" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="31" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:A17">
-    <cfRule type="beginsWith" dxfId="58" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="55" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="57" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="54" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="56" priority="28" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="28" stopIfTrue="1">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="beginsWith" dxfId="55" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="52" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A21,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="54" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="51" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A21,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="53" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="52" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="51" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="20">
       <formula>LEN(TRIM(B21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="beginsWith" dxfId="50" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="47" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="49" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="46" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="48" priority="13" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="47" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="46" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="15">
       <formula>LEN(TRIM(B23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="beginsWith" dxfId="45" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="42" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="44" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="41" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="43" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="42" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="41" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="10">
       <formula>LEN(TRIM(B25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="beginsWith" dxfId="40" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="37" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A24,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="39" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="36" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A24,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="38" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="37" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="36" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="5">
       <formula>LEN(TRIM(B24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3332,7 +3310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37D3F2F-6FA3-E945-A3ED-EFC8DABE8040}">
   <dimension ref="A1:AAA22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -3345,132 +3323,132 @@
   <sheetData>
     <row r="1" spans="1:703" ht="19" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703" ht="19" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703" ht="19" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="HA3" s="4"/>
       <c r="AAA3" s="5"/>
     </row>
     <row r="4" spans="1:703" ht="19" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703" ht="19" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703" ht="19" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703" ht="19" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703" ht="19" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
     <row r="9" spans="1:703" ht="19" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
     <row r="10" spans="1:703" ht="19" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:703" ht="19" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:703" ht="19" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:703" ht="19" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:703" ht="19" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:703" ht="19" customHeight="1">
@@ -3478,10 +3456,17 @@
         <v>9</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:703" ht="19" customHeight="1"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:703" ht="19" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="17" ht="19" customHeight="1"/>
     <row r="18" ht="19" customHeight="1"/>
     <row r="19" ht="19" customHeight="1"/>
@@ -3494,59 +3479,59 @@
     <sortCondition ref="A1:A15"/>
   </sortState>
   <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="35" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="32" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="34" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="31" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="33" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="32" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="31" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="18">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="beginsWith" dxfId="30" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="27" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A11,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="29" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="26" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A11,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="28" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="expression" dxfId="27" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="26" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="13">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A10">
-    <cfRule type="beginsWith" dxfId="25" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="22" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="21" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="23" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B10">
-    <cfRule type="expression" dxfId="22" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="21" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3559,7 +3544,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CC5913-9CC1-104B-A93C-2AE9134DFE8B}">
   <dimension ref="A1:AAA35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -3572,80 +3559,80 @@
   <sheetData>
     <row r="1" spans="1:703" ht="19" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703" ht="19" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703" ht="19" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="HA3" s="4"/>
       <c r="AAA3" s="5"/>
     </row>
     <row r="4" spans="1:703" ht="19" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703" ht="19" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703" ht="19" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703" ht="19" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703" ht="19" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:703" ht="19" customHeight="1">
@@ -3658,58 +3645,58 @@
     </row>
     <row r="10" spans="1:703" ht="19" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:703" ht="19" customHeight="1">
       <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:703" ht="19" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:703" ht="19" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:703" ht="19" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:703" ht="19" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:703" ht="19" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" ht="19" customHeight="1"/>
@@ -3777,225 +3764,225 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="HA10" s="4"/>
       <c r="AAA10" s="5"/>
     </row>
     <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:703">
       <c r="A12" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:703">
       <c r="A13" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:703">
       <c r="A14" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:703">
       <c r="A15" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:703">
       <c r="A16" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[base] - `clear(vars)`: improve output/console messages. No change in functionality/logic.
[web]
- `checkAll(locator)`: **NEW** command to "check" all matching CheckBox web elements.
- `uncheckAll(locator)`: **NEW** command to "uncheck" all matching CheckBox web elements.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-03.data.xlsx
+++ b/artifact/data/web-03.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10806"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4375CCD1-33C6-174A-A6EF-ED881E4003E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F593B2-BACE-2B47-B42A-54DDD0F838D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="6840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25580" windowHeight="10980" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -21,9 +21,10 @@
     <sheet name="locators-name" sheetId="7" r:id="rId6"/>
     <sheet name="locators-css" sheetId="4" r:id="rId7"/>
     <sheet name="locators-xpath" sheetId="8" r:id="rId8"/>
+    <sheet name="locators-xpath2" sheetId="10" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="227">
   <si>
     <t>true</t>
   </si>
@@ -647,6 +648,102 @@
   </si>
   <si>
     <t>500</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/goldbox/</t>
+  </si>
+  <si>
+    <t>app.url</t>
+  </si>
+  <si>
+    <t>app.pageTitle.loc</t>
+  </si>
+  <si>
+    <t>class=gbh1-bold</t>
+  </si>
+  <si>
+    <t>app.pageTitle.text</t>
+  </si>
+  <si>
+    <t>Today's Deals</t>
+  </si>
+  <si>
+    <t>app.title</t>
+  </si>
+  <si>
+    <t>Gold Box Deals | Today's Deals - Amazon.com</t>
+  </si>
+  <si>
+    <t>app.back2top.loc</t>
+  </si>
+  <si>
+    <t>app.back2top.text</t>
+  </si>
+  <si>
+    <t>Back to top</t>
+  </si>
+  <si>
+    <t>app.amzLinks.loc</t>
+  </si>
+  <si>
+    <t>//table[contains(@class, "navFooterMoreOnAmazon")]//td[contains(@class,"navFooterDescItem")]/a[starts-with(text(),"Amazon")]</t>
+  </si>
+  <si>
+    <t>app.amzLinks.count</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>app.filter.loc</t>
+  </si>
+  <si>
+    <t>id=widgetFilters</t>
+  </si>
+  <si>
+    <t>app.availability-checkboxes.loc</t>
+  </si>
+  <si>
+    <t>//div[@id="navFooter"]/a[@href="#nav-top"]//span[contains(@class,"navFooterBackToTopText")]</t>
+  </si>
+  <si>
+    <t>app.availability-checkboxes.active.loc</t>
+  </si>
+  <si>
+    <t>app.availability.loc</t>
+  </si>
+  <si>
+    <t>//*[@id='widgetFilters']//div[./*[normalize-space(text())="Availability"]]</t>
+  </si>
+  <si>
+    <t>${app.availability.loc}//following::input[@type='checkbox']</t>
+  </si>
+  <si>
+    <t>${app.availability.loc}//following::label[normalize-space(.//text())='Active']/input[@type='checkbox']</t>
+  </si>
+  <si>
+    <t>app.avgCustReview.loc</t>
+  </si>
+  <si>
+    <t>//*[@id='widgetFilters']//div[./*[normalize-space(text())="Avg. Customer Review"]]</t>
+  </si>
+  <si>
+    <t>app.avgCustReview.4star.loc</t>
+  </si>
+  <si>
+    <t>${app.avgCustReview.loc}//following::a[ .//*[contains(@class,'a-star-4')] and .//span[normalize-space(text()) = '&amp; Up']]</t>
+  </si>
+  <si>
+    <t>product keyword</t>
+  </si>
+  <si>
+    <t>Tablet</t>
+  </si>
+  <si>
+    <t>product max price</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -789,7 +886,267 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="100">
+  <dxfs count="120">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2371,7 +2728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -2523,40 +2882,40 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1 A3:A9 A22:A1048576">
-    <cfRule type="beginsWith" dxfId="99" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="119" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="98" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="118" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="97" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="117" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1 B3:B9 B22:B1048576">
-    <cfRule type="expression" dxfId="96" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="95" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="115" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="beginsWith" dxfId="94" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="114" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="93" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="113" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="92" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="112" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="91" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="90" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="110" priority="5">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2674,21 +3033,21 @@
     <sortCondition ref="A1:A9"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="89" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="109" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="88" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="108" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="87" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="107" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="86" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="85" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="105" priority="12">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2775,40 +3134,40 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="84" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="104" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="83" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="103" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="82" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="102" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="81" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="80" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="100" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A12">
-    <cfRule type="beginsWith" dxfId="79" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="99" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="78" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="98" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="77" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="97" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B12">
-    <cfRule type="expression" dxfId="76" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="75" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="95" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2897,32 +3256,32 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="beginsWith" dxfId="74" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="94" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="73" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="93" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="72" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="92" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="71" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="70" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="90" priority="13">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="beginsWith" dxfId="69" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="89" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="68" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="88" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="67" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="87" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3174,130 +3533,130 @@
     <sortCondition ref="A17:A25"/>
   </sortState>
   <conditionalFormatting sqref="A18:A20 A22 A26:A1048576 A1:A13">
-    <cfRule type="beginsWith" dxfId="66" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="86" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="65" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="85" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="64" priority="42" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="84" priority="42" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 B10:B13 B22 B26:B1048576 B1:B8">
-    <cfRule type="expression" dxfId="63" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="43" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="62" priority="44">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="44">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="61" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="81" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="60" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="80" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="59" priority="34" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="34" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="beginsWith" dxfId="58" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="78" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="57" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="77" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="56" priority="31" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="76" priority="31" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:A17">
-    <cfRule type="beginsWith" dxfId="55" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="75" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="54" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="74" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="53" priority="28" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="28" stopIfTrue="1">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="beginsWith" dxfId="52" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="72" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A21,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="51" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="71" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A21,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="50" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="49" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="48" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="20">
       <formula>LEN(TRIM(B21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="beginsWith" dxfId="47" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="67" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="66" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="45" priority="13" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="44" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="43" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="15">
       <formula>LEN(TRIM(B23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="beginsWith" dxfId="42" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="62" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="41" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="61" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="40" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="39" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="38" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="10">
       <formula>LEN(TRIM(B25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="beginsWith" dxfId="37" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="57" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A24,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="36" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="56" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A24,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="35" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="34" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="33" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="5">
       <formula>LEN(TRIM(B24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3310,7 +3669,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37D3F2F-6FA3-E945-A3ED-EFC8DABE8040}">
   <dimension ref="A1:AAA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -3479,59 +3840,59 @@
     <sortCondition ref="A1:A15"/>
   </sortState>
   <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="32" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="52" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="31" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="51" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="30" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="29" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="28" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="18">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="beginsWith" dxfId="27" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="47" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A11,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="46" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A11,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="25" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="expression" dxfId="24" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="23" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="13">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A10">
-    <cfRule type="beginsWith" dxfId="22" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="42" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="21" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="41" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="20" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B10">
-    <cfRule type="expression" dxfId="19" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3724,21 +4085,21 @@
     <sortCondition ref="A1:A16"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="17" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="37" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="36" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="15" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="14" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="13" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3751,7 +4112,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938A5DF5-858F-F04F-A650-D78F3893CC59}">
   <dimension ref="A1:AAA25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -3991,52 +4354,322 @@
     <sortCondition ref="A1:A25"/>
   </sortState>
   <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="beginsWith" dxfId="12" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="32" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="11" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="31" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B1048576 B13:B14">
-    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="8" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="13">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="beginsWith" dxfId="7" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="27" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="26" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B13">
-    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="22" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="21" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15D721F-E928-8949-A67C-84C364E740E7}">
+  <dimension ref="A1:AAA36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="33" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="103.1640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703" ht="22" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703" ht="22" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703" ht="22" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
+    </row>
+    <row r="4" spans="1:703" ht="22" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703" ht="22" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703" ht="22" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703" ht="22" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703" ht="22" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703" ht="22" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+    <row r="10" spans="1:703" ht="22" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="HA10" s="4"/>
+      <c r="AAA10" s="5"/>
+    </row>
+    <row r="11" spans="1:703" ht="22" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="HA11" s="4"/>
+      <c r="AAA11" s="5"/>
+    </row>
+    <row r="12" spans="1:703" ht="22" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:703" ht="22" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:703" ht="22" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:703" ht="22" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="16" spans="1:703" ht="22" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="17" ht="22" customHeight="1"/>
+    <row r="18" ht="22" customHeight="1"/>
+    <row r="19" ht="22" customHeight="1"/>
+    <row r="20" ht="22" customHeight="1"/>
+    <row r="21" ht="22" customHeight="1"/>
+    <row r="22" ht="22" customHeight="1"/>
+    <row r="23" ht="22" customHeight="1"/>
+    <row r="24" ht="22" customHeight="1"/>
+    <row r="25" ht="22" customHeight="1"/>
+    <row r="26" ht="22" customHeight="1"/>
+    <row r="27" ht="22" customHeight="1"/>
+    <row r="28" ht="22" customHeight="1"/>
+    <row r="29" ht="22" customHeight="1"/>
+    <row r="30" ht="22" customHeight="1"/>
+    <row r="31" ht="22" customHeight="1"/>
+    <row r="32" ht="22" customHeight="1"/>
+    <row r="33" ht="22" customHeight="1"/>
+    <row r="34" ht="22" customHeight="1"/>
+    <row r="35" ht="22" customHeight="1"/>
+    <row r="36" ht="22" customHeight="1"/>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A16:A1048576">
+    <cfRule type="beginsWith" dxfId="19" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="18" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="17" priority="18" stopIfTrue="1">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:B1048576 B14:B15">
+    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="15" priority="20">
+      <formula>LEN(TRIM(B14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A9 A11:A14">
+    <cfRule type="beginsWith" dxfId="14" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="13" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B9 B11:B12 B14">
+    <cfRule type="expression" dxfId="11" priority="14" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="10" priority="15">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="beginsWith" dxfId="9" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="8" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="7" priority="10" stopIfTrue="1">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="beginsWith" dxfId="6" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A10,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="5" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A10,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5" stopIfTrue="1">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="2" priority="7">
+      <formula>LEN(TRIM(B10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
+      <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- [CSV `excel(file,sheet,startCell)`](../expressions/CSVexpression.md#excel): **NEW** operation to import CSV into   a Excel worksheet. By default, `startCell` is set to `A1`.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-03.data.xlsx
+++ b/artifact/data/web-03.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F593B2-BACE-2B47-B42A-54DDD0F838D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAD8487-1C71-6B41-85AC-4E76EC9C7B21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25580" windowHeight="10980" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="10520" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="246">
   <si>
     <t>true</t>
   </si>
@@ -744,6 +744,63 @@
   </si>
   <si>
     <t>30</t>
+  </si>
+  <si>
+    <t>product min review</t>
+  </si>
+  <si>
+    <t>//[@id='${deal.item.id}']</t>
+  </si>
+  <si>
+    <t>deal.container.loc</t>
+  </si>
+  <si>
+    <t>deal.item.loc</t>
+  </si>
+  <si>
+    <t>deal.price.loc</t>
+  </si>
+  <si>
+    <t>deal.endsIn.loc</t>
+  </si>
+  <si>
+    <t>deal.title.loc</t>
+  </si>
+  <si>
+    <t>deal.soldBy.loc</t>
+  </si>
+  <si>
+    <t>deal.reviewCount.loc</t>
+  </si>
+  <si>
+    <t>//*[@id='${deal.item.id}']//*[contains(@class,'priceBlock')]</t>
+  </si>
+  <si>
+    <t>//*[@id='${deal.item.id}']//*[@id='${deal.item.id}_dealClock']</t>
+  </si>
+  <si>
+    <t>//*[@id='${deal.item.id}']//*[@id='dealTitle']</t>
+  </si>
+  <si>
+    <t>//*[@id='${deal.item.id}']//*[@id='shipSoldInfo']</t>
+  </si>
+  <si>
+    <t>//*[@id='${deal.item.id}']//*[contains(@class,'reviewStars')]//*[contains(@class,'a-color-base')]</t>
+  </si>
+  <si>
+    <t>deal.nextPage.loc</t>
+  </si>
+  <si>
+    <t>//div[@id='FilterItemView_page_pagination']//span[@class='a-declarative']/div[not(contains(@class,'hidden'))]/*[contains(@class,'a-pagination')]/*[@class='a-last']</t>
+  </si>
+  <si>
+    <t>deal.filterSummary.loc</t>
+  </si>
+  <si>
+    <t>//*[@id='FilterItemView_all_summary']/div</t>
+  </si>
+  <si>
+    <t>//*[contains(@class,'widgetContainer')]//*[@id='widgetContent']//*[contains(@class,'tallCellView')]</t>
   </si>
 </sst>
 </file>
@@ -886,7 +943,72 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="120">
+  <dxfs count="125">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2882,40 +3004,40 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1 A3:A9 A22:A1048576">
-    <cfRule type="beginsWith" dxfId="119" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="124" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="118" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="123" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="117" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="122" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1 B3:B9 B22:B1048576">
-    <cfRule type="expression" dxfId="116" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="115" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="120" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="beginsWith" dxfId="114" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="119" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="113" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="118" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="112" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="117" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="111" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="110" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="115" priority="5">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3033,21 +3155,21 @@
     <sortCondition ref="A1:A9"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="109" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="114" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="108" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="113" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="107" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="112" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="106" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="105" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="110" priority="12">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3134,40 +3256,40 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="104" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="109" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="103" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="108" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="102" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="107" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="101" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="100" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="105" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A12">
-    <cfRule type="beginsWith" dxfId="99" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="104" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="98" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="103" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="97" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="102" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B12">
-    <cfRule type="expression" dxfId="96" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="95" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="100" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3256,32 +3378,32 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="beginsWith" dxfId="94" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="99" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="93" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="98" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="92" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="97" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="91" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="90" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="95" priority="13">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="beginsWith" dxfId="89" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="94" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="88" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="93" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="87" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="92" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3533,130 +3655,130 @@
     <sortCondition ref="A17:A25"/>
   </sortState>
   <conditionalFormatting sqref="A18:A20 A22 A26:A1048576 A1:A13">
-    <cfRule type="beginsWith" dxfId="86" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="91" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="85" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="90" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="84" priority="42" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="89" priority="42" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 B10:B13 B22 B26:B1048576 B1:B8">
-    <cfRule type="expression" dxfId="83" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="43" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="82" priority="44">
+    <cfRule type="notContainsBlanks" dxfId="87" priority="44">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="81" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="86" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="80" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="85" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="79" priority="34" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="84" priority="34" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="beginsWith" dxfId="78" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="83" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="77" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="82" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="76" priority="31" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="81" priority="31" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:A17">
-    <cfRule type="beginsWith" dxfId="75" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="80" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="74" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="79" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="73" priority="28" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="28" stopIfTrue="1">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="beginsWith" dxfId="72" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="77" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A21,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="71" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="76" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A21,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="70" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="69" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="68" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="20">
       <formula>LEN(TRIM(B21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="beginsWith" dxfId="67" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="72" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="66" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="71" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="65" priority="13" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="64" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="63" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="15">
       <formula>LEN(TRIM(B23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="beginsWith" dxfId="62" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="67" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="61" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="66" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="60" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="59" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="58" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="10">
       <formula>LEN(TRIM(B25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="beginsWith" dxfId="57" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="62" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A24,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="56" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="61" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A24,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="55" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="54" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="53" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="5">
       <formula>LEN(TRIM(B24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3840,59 +3962,59 @@
     <sortCondition ref="A1:A15"/>
   </sortState>
   <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="52" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="57" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="51" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="56" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="50" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="49" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="48" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="18">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="beginsWith" dxfId="47" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="52" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A11,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="51" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A11,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="45" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="expression" dxfId="44" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="43" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="13">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A10">
-    <cfRule type="beginsWith" dxfId="42" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="47" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="41" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="46" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="40" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B10">
-    <cfRule type="expression" dxfId="39" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="38" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4085,21 +4207,21 @@
     <sortCondition ref="A1:A16"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="37" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="42" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="36" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="41" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="35" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="34" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="33" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4354,51 +4476,51 @@
     <sortCondition ref="A1:A25"/>
   </sortState>
   <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="beginsWith" dxfId="32" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="37" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="31" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="36" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="30" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B1048576 B13:B14">
-    <cfRule type="expression" dxfId="29" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="28" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="13">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="beginsWith" dxfId="27" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="32" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="31" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="25" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B13">
-    <cfRule type="expression" dxfId="24" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="23" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="22" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="27" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="21" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="26" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="20" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4409,10 +4531,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15D721F-E928-8949-A67C-84C364E740E7}">
-  <dimension ref="A1:AAA36"/>
+  <dimension ref="A1:AAA34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -4574,102 +4696,189 @@
         <v>226</v>
       </c>
     </row>
-    <row r="17" ht="22" customHeight="1"/>
-    <row r="18" ht="22" customHeight="1"/>
-    <row r="19" ht="22" customHeight="1"/>
-    <row r="20" ht="22" customHeight="1"/>
-    <row r="21" ht="22" customHeight="1"/>
-    <row r="22" ht="22" customHeight="1"/>
-    <row r="23" ht="22" customHeight="1"/>
-    <row r="24" ht="22" customHeight="1"/>
-    <row r="25" ht="22" customHeight="1"/>
-    <row r="26" ht="22" customHeight="1"/>
-    <row r="27" ht="22" customHeight="1"/>
-    <row r="28" ht="22" customHeight="1"/>
-    <row r="29" ht="22" customHeight="1"/>
-    <row r="30" ht="22" customHeight="1"/>
-    <row r="31" ht="22" customHeight="1"/>
-    <row r="32" ht="22" customHeight="1"/>
+    <row r="17" spans="1:2" ht="22" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="22" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="22" customHeight="1">
+      <c r="A19" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="22" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="22" customHeight="1">
+      <c r="A21" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="22" customHeight="1">
+      <c r="A22" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="22" customHeight="1">
+      <c r="A23" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="22" customHeight="1">
+      <c r="A24" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="22" customHeight="1">
+      <c r="A25" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="22" customHeight="1">
+      <c r="A26" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="22" customHeight="1"/>
+    <row r="28" spans="1:2" ht="22" customHeight="1"/>
+    <row r="29" spans="1:2" ht="22" customHeight="1"/>
+    <row r="30" spans="1:2" ht="22" customHeight="1"/>
+    <row r="31" spans="1:2" ht="22" customHeight="1"/>
+    <row r="32" spans="1:2" ht="22" customHeight="1"/>
     <row r="33" ht="22" customHeight="1"/>
     <row r="34" ht="22" customHeight="1"/>
-    <row r="35" ht="22" customHeight="1"/>
-    <row r="36" ht="22" customHeight="1"/>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A16:A1048576">
+  <conditionalFormatting sqref="A22:A1048576 A16:A19">
+    <cfRule type="beginsWith" dxfId="24" priority="21" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="23" priority="22" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="22" priority="23" stopIfTrue="1">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:B15 B22:B1048576 B17:B19">
+    <cfRule type="expression" dxfId="21" priority="24" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="20" priority="25">
+      <formula>LEN(TRIM(B14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A9 A11:A14">
     <cfRule type="beginsWith" dxfId="19" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="18" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="17" priority="18" stopIfTrue="1">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
+      <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:B1048576 B14:B15">
+  <conditionalFormatting sqref="B1:B9 B11:B12 B14">
     <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="15" priority="20">
-      <formula>LEN(TRIM(B14))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A9 A11:A14">
-    <cfRule type="beginsWith" dxfId="14" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="13" stopIfTrue="1">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B9 B11:B12 B14">
-    <cfRule type="expression" dxfId="11" priority="14" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="15">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="beginsWith" dxfId="9" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="14" priority="13" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="13" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="15" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="beginsWith" dxfId="6" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="11" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A10,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="5" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="10" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A10,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(A10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="12">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="7">
       <formula>LEN(TRIM(B13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:A21">
+    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A20,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A20,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20:B21">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
+      <formula>LEN(TRIM(B20))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[web] - [`nexial.web.highlight`]: renamed from the previous `nexial.highlight` System variable (which is still working) for consistency and clearer namespacing. - [`nexial.web.highlight.waitMs`]: renamed from the previous `nexial.highlightWaitMs` (which is still working) for consistency and clearer namespacing. - [`nexial.web.highlight.style`]: **NEW** System variable to allow for customization of web element highlighting, which is assumed as CSS style. The default is `background:#faf557;`.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-03.data.xlsx
+++ b/artifact/data/web-03.data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAD8487-1C71-6B41-85AC-4E76EC9C7B21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFD8BD1-2A44-6546-B3F9-48EED1CF8273}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="10520" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,6 +45,7 @@
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="264">
   <si>
     <t>true</t>
   </si>
@@ -728,27 +729,6 @@
     <t>//*[@id='widgetFilters']//div[./*[normalize-space(text())="Avg. Customer Review"]]</t>
   </si>
   <si>
-    <t>app.avgCustReview.4star.loc</t>
-  </si>
-  <si>
-    <t>${app.avgCustReview.loc}//following::a[ .//*[contains(@class,'a-star-4')] and .//span[normalize-space(text()) = '&amp; Up']]</t>
-  </si>
-  <si>
-    <t>product keyword</t>
-  </si>
-  <si>
-    <t>Tablet</t>
-  </si>
-  <si>
-    <t>product max price</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>product min review</t>
-  </si>
-  <si>
     <t>//[@id='${deal.item.id}']</t>
   </si>
   <si>
@@ -773,9 +753,6 @@
     <t>deal.reviewCount.loc</t>
   </si>
   <si>
-    <t>//*[@id='${deal.item.id}']//*[contains(@class,'priceBlock')]</t>
-  </si>
-  <si>
     <t>//*[@id='${deal.item.id}']//*[@id='${deal.item.id}_dealClock']</t>
   </si>
   <si>
@@ -801,6 +778,84 @@
   </si>
   <si>
     <t>//*[contains(@class,'widgetContainer')]//*[@id='widgetContent']//*[contains(@class,'tallCellView')]</t>
+  </si>
+  <si>
+    <t>//*[@id='${deal.item.id}']//*[contains(@class,'priceBlock')]/span</t>
+  </si>
+  <si>
+    <t>deal.link.loc</t>
+  </si>
+  <si>
+    <t>//*[@id='${deal.item.id}']//a[@id='dealImage']</t>
+  </si>
+  <si>
+    <t>deal.thumbnail.loc</t>
+  </si>
+  <si>
+    <t>//*[@id='${deal.item.id}']//a[@id='dealImage']//img</t>
+  </si>
+  <si>
+    <t>desired max price</t>
+  </si>
+  <si>
+    <t>desired min review</t>
+  </si>
+  <si>
+    <t>desire product keywords</t>
+  </si>
+  <si>
+    <t>nexial.breakCurrentIteration</t>
+  </si>
+  <si>
+    <t>Tablet|TV|Echo|phone|Monoxide</t>
+  </si>
+  <si>
+    <t>deal.output.file</t>
+  </si>
+  <si>
+    <t>$(syspath|out|fullpath)/mydeals.html</t>
+  </si>
+  <si>
+    <t>deal.item.template</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/deal-item.html</t>
+  </si>
+  <si>
+    <t>desired review stars</t>
+  </si>
+  <si>
+    <t>${app.avgCustReview.loc}//following::a[ .//*[contains(@class,'a-star-${desired review stars}')] and .//span[normalize-space(text()) = '&amp; Up']]</t>
+  </si>
+  <si>
+    <t>app.avgCustReview.stars.loc</t>
+  </si>
+  <si>
+    <t>deal.output.header</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/deals.header.html</t>
+  </si>
+  <si>
+    <t>deal.output.footer</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/deals.footer.html</t>
+  </si>
+  <si>
+    <t>nexial.stepByStep</t>
+  </si>
+  <si>
+    <t>nexial.inspectOnPause</t>
+  </si>
+  <si>
+    <t>nexial.browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>200</t>
   </si>
 </sst>
 </file>
@@ -2851,7 +2906,7 @@
   <dimension ref="A1:AAA21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -4531,10 +4586,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15D721F-E928-8949-A67C-84C364E740E7}">
-  <dimension ref="A1:AAA34"/>
+  <dimension ref="A1:AAA38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -4674,130 +4729,218 @@
     </row>
     <row r="14" spans="1:703" ht="22" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>221</v>
+        <v>254</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="1:703" ht="22" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>223</v>
+        <v>252</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>224</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:703" ht="22" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>226</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="22" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>194</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="22" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>245</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="22" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="22" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="22" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="22" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="22" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="22" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="22" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="22" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="22" customHeight="1"/>
-    <row r="28" spans="1:2" ht="22" customHeight="1"/>
-    <row r="29" spans="1:2" ht="22" customHeight="1"/>
-    <row r="30" spans="1:2" ht="22" customHeight="1"/>
-    <row r="31" spans="1:2" ht="22" customHeight="1"/>
-    <row r="32" spans="1:2" ht="22" customHeight="1"/>
-    <row r="33" ht="22" customHeight="1"/>
-    <row r="34" ht="22" customHeight="1"/>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="22" customHeight="1">
+      <c r="A27" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="22" customHeight="1">
+      <c r="A28" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="22" customHeight="1">
+      <c r="A29" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="22" customHeight="1">
+      <c r="A30" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="22" customHeight="1">
+      <c r="A31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="22" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="22" customHeight="1">
+      <c r="A33" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="22" customHeight="1">
+      <c r="A34" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="22" customHeight="1">
+      <c r="A35" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A22:A1048576 A16:A19">
+  <conditionalFormatting sqref="A17:A20 A23:A1048576">
     <cfRule type="beginsWith" dxfId="24" priority="21" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A17,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="23" priority="22" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A17,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="22" priority="23" stopIfTrue="1">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
+      <formula>LEN(TRIM(A17))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:B15 B22:B1048576 B17:B19">
+  <conditionalFormatting sqref="B14:B16 B18:B20 B23:B1048576">
     <cfRule type="expression" dxfId="21" priority="24" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
@@ -4805,7 +4948,7 @@
       <formula>LEN(TRIM(B14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A9 A11:A14">
+  <conditionalFormatting sqref="A1:A9 A11:A15">
     <cfRule type="beginsWith" dxfId="19" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
@@ -4816,7 +4959,7 @@
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B9 B11:B12 B14">
+  <conditionalFormatting sqref="B1:B9 B11:B12 B14:B15">
     <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
@@ -4824,15 +4967,15 @@
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
+  <conditionalFormatting sqref="A16">
     <cfRule type="beginsWith" dxfId="14" priority="13" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="13" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="12" priority="15" stopIfTrue="1">
-      <formula>LEN(TRIM(A15))&gt;0</formula>
+      <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
@@ -4862,23 +5005,23 @@
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:A21">
+  <conditionalFormatting sqref="A21:A22">
     <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A20,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A21,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A20,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A21,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
+      <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20:B21">
+  <conditionalFormatting sqref="B21:B22">
     <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="5">
-      <formula>LEN(TRIM(B20))&gt;0</formula>
+      <formula>LEN(TRIM(B21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[built-in functions] - fixed wrong references in `$(syspath|script)`
[web]
- shipped with Selenium 3.14.0
- improve log messages (console) over FAIL conditions
- support page load time out
- graceful passthrough when `open()` takes longer than expected to load page due to external links

[rdbms]
- support reading of file content when execution `runSQL()` and `saveResult()` commands

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-03.data.xlsx
+++ b/artifact/data/web-03.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCFC04A-DAC2-C641-B1B1-27A6F0FD1ACB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBF8BCD-72EF-3D40-80B4-D8F0C3027EA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="10520" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="31560" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,6 @@
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -58,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="277">
   <si>
     <t>true</t>
   </si>
@@ -846,9 +845,6 @@
     <t>desired product keywords</t>
   </si>
   <si>
-    <t>Tablet|TV|Echo|phone|Phone|Gear|toy|Toy|Game|game</t>
-  </si>
-  <si>
     <t>$(syspath|data|fullpath)/deals.item.html</t>
   </si>
   <si>
@@ -871,6 +867,33 @@
   </si>
   <si>
     <t>//div[@id='FilterItemView_page_pagination']//span[@class='a-declarative']/div[not(contains(@class,'hidden'))]/*[contains(@class,'a-pagination')]/*[@class='a-last']/a</t>
+  </si>
+  <si>
+    <t>//nexial.pollWaitMs</t>
+  </si>
+  <si>
+    <t>nexial.web.pageLoadWaitMs</t>
+  </si>
+  <si>
+    <t>//nexial.enforcePageSourceStability</t>
+  </si>
+  <si>
+    <t>//nexial.web.alwaysWait</t>
+  </si>
+  <si>
+    <t>TABLET|TV|ECHO|PHONE|GEAR|TOY|GAME|MUSIC|LAPTOP|SPEAKER|CABLE|SAMSUNG|MONITOR|WIRE|USB|MOUNT|HD</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>nexial.browser.windowSize</t>
+  </si>
+  <si>
+    <t>1920x1280</t>
+  </si>
+  <si>
+    <t>3000</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1036,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="145">
+  <dxfs count="153">
     <dxf>
       <font>
         <b/>
@@ -1601,43 +1624,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2288,117 +2274,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2501,6 +2376,80 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2566,6 +2515,43 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2886,6 +2872,155 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3181,7 +3316,7 @@
   <dimension ref="A1:AAA21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -3334,40 +3469,40 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1 A3:A9 A22:A1048576">
-    <cfRule type="beginsWith" dxfId="144" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="146" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="143" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="145" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="142" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="144" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1 B3:B9 B22:B1048576">
-    <cfRule type="expression" dxfId="141" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="140" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="142" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="beginsWith" dxfId="139" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="141" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="138" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="140" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="137" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="139" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="136" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="135" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="137" priority="5">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3485,21 +3620,21 @@
     <sortCondition ref="A1:A9"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="134" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="136" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="133" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="135" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="132" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="134" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="131" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="130" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="132" priority="12">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3586,40 +3721,40 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="129" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="131" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="128" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="130" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="127" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="129" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="126" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="125" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="127" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A12">
-    <cfRule type="beginsWith" dxfId="124" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="126" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="123" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="125" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="122" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="124" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B12">
-    <cfRule type="expression" dxfId="121" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="120" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="122" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3708,32 +3843,32 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="beginsWith" dxfId="119" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="121" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="118" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="120" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="117" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="119" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="116" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="115" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="117" priority="13">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="beginsWith" dxfId="114" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="116" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="113" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="115" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="112" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="114" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3985,130 +4120,130 @@
     <sortCondition ref="A17:A25"/>
   </sortState>
   <conditionalFormatting sqref="A18:A20 A22 A26:A1048576 A1:A13">
-    <cfRule type="beginsWith" dxfId="111" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="113" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="110" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="112" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="109" priority="42" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="111" priority="42" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 B10:B13 B22 B26:B1048576 B1:B8">
-    <cfRule type="expression" dxfId="108" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="43" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="107" priority="44">
+    <cfRule type="notContainsBlanks" dxfId="109" priority="44">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="106" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="108" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="105" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="107" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="104" priority="34" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="106" priority="34" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="beginsWith" dxfId="103" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="105" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="102" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="104" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="101" priority="31" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="103" priority="31" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:A17">
-    <cfRule type="beginsWith" dxfId="100" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="102" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="99" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="101" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="98" priority="28" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="100" priority="28" stopIfTrue="1">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="beginsWith" dxfId="97" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="99" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A21,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="96" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="98" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A21,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="95" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="97" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="94" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="93" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="95" priority="20">
       <formula>LEN(TRIM(B21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="beginsWith" dxfId="92" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="94" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="91" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="93" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="90" priority="13" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="92" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="89" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="88" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="90" priority="15">
       <formula>LEN(TRIM(B23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="beginsWith" dxfId="87" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="89" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="86" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="88" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="85" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="87" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="84" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="83" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="85" priority="10">
       <formula>LEN(TRIM(B25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="beginsWith" dxfId="82" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="84" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A24,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="81" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="83" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A24,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="80" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="82" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="79" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="78" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="5">
       <formula>LEN(TRIM(B24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4122,7 +4257,7 @@
   <dimension ref="A1:AAA22"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -4292,59 +4427,59 @@
     <sortCondition ref="A1:A15"/>
   </sortState>
   <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="77" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="79" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="76" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="78" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="75" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="74" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="73" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="18">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="beginsWith" dxfId="72" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="74" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A11,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="71" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="73" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A11,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="70" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="expression" dxfId="69" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="68" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="13">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A10">
-    <cfRule type="beginsWith" dxfId="67" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="69" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="66" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="68" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="65" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B10">
-    <cfRule type="expression" dxfId="64" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="63" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4357,8 +4492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CC5913-9CC1-104B-A93C-2AE9134DFE8B}">
   <dimension ref="A1:AAA35"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -4537,21 +4672,21 @@
     <sortCondition ref="A1:A16"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="62" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="64" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="61" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="63" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="60" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="59" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="58" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4564,8 +4699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938A5DF5-858F-F04F-A650-D78F3893CC59}">
   <dimension ref="A1:AAA25"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -4806,51 +4941,51 @@
     <sortCondition ref="A1:A25"/>
   </sortState>
   <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="beginsWith" dxfId="57" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="59" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="56" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="58" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="55" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B1048576 B13:B14">
-    <cfRule type="expression" dxfId="54" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="53" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="13">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="beginsWith" dxfId="52" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="54" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="51" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="53" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="50" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B13">
-    <cfRule type="expression" dxfId="49" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="48" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="47" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="49" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="48" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="45" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4861,10 +4996,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15D721F-E928-8949-A67C-84C364E740E7}">
-  <dimension ref="A1:AAA41"/>
+  <dimension ref="A1:AAA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -4918,10 +5053,10 @@
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="HA5" s="6"/>
       <c r="AAA5" s="6"/>
@@ -4938,285 +5073,293 @@
     </row>
     <row r="7" spans="1:703" ht="23" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>196</v>
+        <v>271</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>195</v>
+        <v>2</v>
       </c>
       <c r="HA7" s="6"/>
       <c r="AAA7" s="6"/>
     </row>
     <row r="8" spans="1:703" ht="23" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>197</v>
+        <v>270</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>198</v>
+        <v>0</v>
       </c>
       <c r="HA8" s="6"/>
       <c r="AAA8" s="6"/>
     </row>
     <row r="9" spans="1:703" ht="23" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>199</v>
+        <v>268</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>200</v>
+        <v>273</v>
       </c>
       <c r="HA9" s="6"/>
       <c r="AAA9" s="6"/>
     </row>
     <row r="10" spans="1:703" ht="23" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>201</v>
+        <v>269</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="HA10" s="4"/>
-      <c r="AAA10" s="5"/>
+        <v>276</v>
+      </c>
+      <c r="HA10" s="6"/>
+      <c r="AAA10" s="6"/>
     </row>
     <row r="11" spans="1:703" ht="23" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="HA11" s="4"/>
-      <c r="AAA11" s="5"/>
+        <v>195</v>
+      </c>
+      <c r="HA11" s="6"/>
+      <c r="AAA11" s="6"/>
     </row>
     <row r="12" spans="1:703" ht="23" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="HA12" s="4"/>
-      <c r="AAA12" s="5"/>
+        <v>198</v>
+      </c>
+      <c r="HA12" s="6"/>
+      <c r="AAA12" s="6"/>
     </row>
     <row r="13" spans="1:703" ht="23" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="HA13" s="4"/>
-      <c r="AAA13" s="5"/>
+        <v>200</v>
+      </c>
+      <c r="HA13" s="6"/>
+      <c r="AAA13" s="6"/>
     </row>
     <row r="14" spans="1:703" ht="23" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="HA14" s="4"/>
       <c r="AAA14" s="5"/>
     </row>
     <row r="15" spans="1:703" ht="23" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="HA15" s="4"/>
       <c r="AAA15" s="5"/>
     </row>
     <row r="16" spans="1:703" ht="23" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="HA16" s="4"/>
       <c r="AAA16" s="5"/>
     </row>
     <row r="17" spans="1:703" ht="23" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="HA17" s="4"/>
       <c r="AAA17" s="5"/>
     </row>
     <row r="18" spans="1:703" ht="23" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>218</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="HA18" s="4"/>
+      <c r="AAA18" s="5"/>
     </row>
     <row r="19" spans="1:703" ht="23" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>220</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="HA19" s="4"/>
+      <c r="AAA19" s="5"/>
     </row>
     <row r="20" spans="1:703" ht="23" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>248</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="HA20" s="4"/>
+      <c r="AAA20" s="5"/>
     </row>
     <row r="21" spans="1:703" ht="23" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>235</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="HA21" s="4"/>
+      <c r="AAA21" s="5"/>
     </row>
     <row r="22" spans="1:703" ht="23" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>263</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:703" ht="23" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:703" ht="23" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>224</v>
+        <v>249</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:703" ht="23" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:703" ht="23" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:703" ht="23" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="1:703" ht="23" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>264</v>
+        <v>224</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>265</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:703" ht="23" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>267</v>
+        <v>225</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>266</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:703" ht="23" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:703" ht="23" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:703" ht="23" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>237</v>
+        <v>263</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>238</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="23" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="23" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="23" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="23" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="23" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="23" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>119</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="23" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>260</v>
@@ -5224,18 +5367,66 @@
     </row>
     <row r="40" spans="1:2" ht="23" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="23" customHeight="1">
       <c r="A41" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="23" customHeight="1">
+      <c r="A42" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="23" customHeight="1">
+      <c r="A43" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="23" customHeight="1">
+      <c r="A44" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="23" customHeight="1">
+      <c r="A45" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>194</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -5243,88 +5434,88 @@
   <sortState ref="A1:B6">
     <sortCondition ref="A1:A6"/>
   </sortState>
-  <conditionalFormatting sqref="A25:A37 A42:A1048576 A21:A22">
+  <conditionalFormatting sqref="A29:A41 A46:A1048576 A25:A26">
     <cfRule type="beginsWith" dxfId="44" priority="49" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A21,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="43" priority="50" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A21,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="42" priority="51" stopIfTrue="1">
-      <formula>LEN(TRIM(A21))&gt;0</formula>
+      <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25:B37 B42:B1048576 B20:B22">
+  <conditionalFormatting sqref="B29:B41 B46:B1048576 B24:B26">
     <cfRule type="expression" dxfId="41" priority="52" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="40" priority="53">
-      <formula>LEN(TRIM(B20))&gt;0</formula>
+      <formula>LEN(TRIM(B24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:A15 A17:A20">
+  <conditionalFormatting sqref="A11:A19 A21:A24">
     <cfRule type="beginsWith" dxfId="39" priority="44" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A7,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A11,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="38" priority="45" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A7,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A11,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="37" priority="46" stopIfTrue="1">
-      <formula>LEN(TRIM(A7))&gt;0</formula>
+      <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:B15 B17:B18 B20">
+  <conditionalFormatting sqref="B11:B19 B21:B22 B24">
     <cfRule type="expression" dxfId="36" priority="47" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="35" priority="48">
-      <formula>LEN(TRIM(B7))&gt;0</formula>
+      <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
+  <conditionalFormatting sqref="A20">
     <cfRule type="beginsWith" dxfId="34" priority="36" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A20,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="33" priority="37" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A20,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="32" priority="38" stopIfTrue="1">
-      <formula>LEN(TRIM(A16))&gt;0</formula>
+      <formula>LEN(TRIM(A20))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
+  <conditionalFormatting sqref="B20">
     <cfRule type="expression" dxfId="31" priority="39" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="30" priority="40">
-      <formula>LEN(TRIM(B16))&gt;0</formula>
+      <formula>LEN(TRIM(B20))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
+  <conditionalFormatting sqref="B23">
     <cfRule type="expression" dxfId="29" priority="34" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="28" priority="35">
-      <formula>LEN(TRIM(B19))&gt;0</formula>
+      <formula>LEN(TRIM(B23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23:A24">
+  <conditionalFormatting sqref="A27:A28">
     <cfRule type="beginsWith" dxfId="27" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="26" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="25" priority="31" stopIfTrue="1">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
+      <formula>LEN(TRIM(A27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23:B24">
+  <conditionalFormatting sqref="B27:B28">
     <cfRule type="expression" dxfId="24" priority="32" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="23" priority="33">
-      <formula>LEN(TRIM(B23))&gt;0</formula>
+      <formula>LEN(TRIM(B27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A4">
@@ -5346,7 +5537,7 @@
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A6">
+  <conditionalFormatting sqref="A5:A10">
     <cfRule type="beginsWith" dxfId="17" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A5,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
@@ -5357,7 +5548,7 @@
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B6">
+  <conditionalFormatting sqref="B5:B10">
     <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
@@ -5365,53 +5556,53 @@
       <formula>LEN(TRIM(B5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40:A41">
+  <conditionalFormatting sqref="A44:A45">
     <cfRule type="beginsWith" dxfId="12" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A40,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A44,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="11" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A40,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A44,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="10" priority="11" stopIfTrue="1">
-      <formula>LEN(TRIM(A40))&gt;0</formula>
+      <formula>LEN(TRIM(A44))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38:B39 B41">
+  <conditionalFormatting sqref="B42:B43 B45">
     <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="8" priority="13">
-      <formula>LEN(TRIM(B38))&gt;0</formula>
+      <formula>LEN(TRIM(B42))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
+  <conditionalFormatting sqref="A42">
     <cfRule type="beginsWith" dxfId="7" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A38,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A42,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="6" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A38,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A42,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="6" stopIfTrue="1">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
+      <formula>LEN(TRIM(A42))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
+  <conditionalFormatting sqref="B42">
     <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="3" priority="8">
-      <formula>LEN(TRIM(B38))&gt;0</formula>
+      <formula>LEN(TRIM(B42))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39">
+  <conditionalFormatting sqref="A43">
     <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A39,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A43,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A39,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A43,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(A39))&gt;0</formula>
+      <formula>LEN(TRIM(A43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- updated amazon deal example - web.checkAll() and web.uncheckAll): added wait time between elements; improved logging
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-03.data.xlsx
+++ b/artifact/data/web-03.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBF8BCD-72EF-3D40-80B4-D8F0C3027EA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE980A37-8077-9B4E-8621-A83C5AF60558}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="31560" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="15780" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="284">
   <si>
     <t>true</t>
   </si>
@@ -719,9 +719,6 @@
     <t>${app.availability.loc}//following::input[@type='checkbox']</t>
   </si>
   <si>
-    <t>${app.availability.loc}//following::label[normalize-space(.//text())='Active']/input[@type='checkbox']</t>
-  </si>
-  <si>
     <t>app.avgCustReview.loc</t>
   </si>
   <si>
@@ -869,9 +866,6 @@
     <t>//div[@id='FilterItemView_page_pagination']//span[@class='a-declarative']/div[not(contains(@class,'hidden'))]/*[contains(@class,'a-pagination')]/*[@class='a-last']/a</t>
   </si>
   <si>
-    <t>//nexial.pollWaitMs</t>
-  </si>
-  <si>
     <t>nexial.web.pageLoadWaitMs</t>
   </si>
   <si>
@@ -884,16 +878,43 @@
     <t>TABLET|TV|ECHO|PHONE|GEAR|TOY|GAME|MUSIC|LAPTOP|SPEAKER|CABLE|SAMSUNG|MONITOR|WIRE|USB|MOUNT|HD</t>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
     <t>nexial.browser.windowSize</t>
   </si>
   <si>
     <t>1920x1280</t>
   </si>
   <si>
-    <t>3000</t>
+    <t>app.availability-checkboxes.checked.loc</t>
+  </si>
+  <si>
+    <t>${app.availability.loc}//following::input[@type='checkbox' and @checked]</t>
+  </si>
+  <si>
+    <t>app.filterSummary.loc</t>
+  </si>
+  <si>
+    <t>nexial.web.highlight</t>
+  </si>
+  <si>
+    <t>nexial.web.highlight.waitMs</t>
+  </si>
+  <si>
+    <t>desired availability type</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>${app.availability.loc}//following::label[normalize-space(.//text())='${desired availability type}']/input[@type='checkbox']</t>
+  </si>
+  <si>
+    <t>//div[@id='FilterItemView_all_summary' and contains(normalize-space(string(.)), '${desired availability type} : ${desired review stars} Stars &amp; Up')]</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>5000</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1057,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="153">
+  <dxfs count="145">
     <dxf>
       <font>
         <b/>
@@ -1624,6 +1645,43 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2274,6 +2332,117 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2376,80 +2545,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2515,43 +2610,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2872,155 +2930,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3469,40 +3378,40 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1 A3:A9 A22:A1048576">
-    <cfRule type="beginsWith" dxfId="146" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="144" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="145" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="143" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="144" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="142" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1 B3:B9 B22:B1048576">
-    <cfRule type="expression" dxfId="143" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="142" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="140" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="beginsWith" dxfId="141" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="139" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="140" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="138" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="139" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="137" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="138" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="137" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="135" priority="5">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3620,21 +3529,21 @@
     <sortCondition ref="A1:A9"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="136" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="134" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="135" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="133" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="134" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="132" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="133" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="132" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="130" priority="12">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3721,40 +3630,40 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="131" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="129" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="130" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="128" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="129" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="127" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="128" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="127" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="125" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A12">
-    <cfRule type="beginsWith" dxfId="126" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="124" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="125" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="123" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="124" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="122" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B12">
-    <cfRule type="expression" dxfId="123" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="122" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="120" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3843,32 +3752,32 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="beginsWith" dxfId="121" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="119" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="120" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="118" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="119" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="117" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="118" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="117" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="115" priority="13">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="beginsWith" dxfId="116" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="114" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="115" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="113" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="114" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="112" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4120,130 +4029,130 @@
     <sortCondition ref="A17:A25"/>
   </sortState>
   <conditionalFormatting sqref="A18:A20 A22 A26:A1048576 A1:A13">
-    <cfRule type="beginsWith" dxfId="113" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="111" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="112" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="110" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="111" priority="42" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="109" priority="42" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 B10:B13 B22 B26:B1048576 B1:B8">
-    <cfRule type="expression" dxfId="110" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="43" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="109" priority="44">
+    <cfRule type="notContainsBlanks" dxfId="107" priority="44">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="108" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="106" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="107" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="105" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="106" priority="34" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="104" priority="34" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="beginsWith" dxfId="105" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="103" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="104" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="102" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="103" priority="31" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="101" priority="31" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:A17">
-    <cfRule type="beginsWith" dxfId="102" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="100" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="101" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="99" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="100" priority="28" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="98" priority="28" stopIfTrue="1">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="beginsWith" dxfId="99" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="97" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A21,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="98" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="96" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A21,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="97" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="95" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="96" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="95" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="93" priority="20">
       <formula>LEN(TRIM(B21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="beginsWith" dxfId="94" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="92" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="93" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="91" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="92" priority="13" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="90" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="91" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="90" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="88" priority="15">
       <formula>LEN(TRIM(B23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="beginsWith" dxfId="89" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="87" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="88" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="86" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="87" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="85" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="86" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="85" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="10">
       <formula>LEN(TRIM(B25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="beginsWith" dxfId="84" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="82" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A24,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="83" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="81" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A24,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="82" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="81" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="80" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="5">
       <formula>LEN(TRIM(B24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4427,59 +4336,59 @@
     <sortCondition ref="A1:A15"/>
   </sortState>
   <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="79" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="77" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="78" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="76" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="77" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="76" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="75" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="18">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="beginsWith" dxfId="74" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="72" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A11,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="73" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="71" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A11,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="72" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="expression" dxfId="71" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="70" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="13">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A10">
-    <cfRule type="beginsWith" dxfId="69" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="67" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="68" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="66" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="67" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B10">
-    <cfRule type="expression" dxfId="66" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="65" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4672,21 +4581,21 @@
     <sortCondition ref="A1:A16"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="64" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="62" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="63" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="61" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="62" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="61" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="60" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4699,8 +4608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938A5DF5-858F-F04F-A650-D78F3893CC59}">
   <dimension ref="A1:AAA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -4941,51 +4850,51 @@
     <sortCondition ref="A1:A25"/>
   </sortState>
   <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="beginsWith" dxfId="59" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="57" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="58" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="56" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="57" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B1048576 B13:B14">
-    <cfRule type="expression" dxfId="56" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="55" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="13">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="beginsWith" dxfId="54" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="52" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="53" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="51" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="52" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B13">
-    <cfRule type="expression" dxfId="51" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="50" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="49" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="47" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="48" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="46" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="47" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4996,15 +4905,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15D721F-E928-8949-A67C-84C364E740E7}">
-  <dimension ref="A1:AAA47"/>
+  <dimension ref="A1:AAA51"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="33" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="103.1640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
@@ -5013,7 +4922,7 @@
   <sheetData>
     <row r="1" spans="1:703" ht="23" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -5023,10 +4932,10 @@
     </row>
     <row r="2" spans="1:703" ht="23" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
@@ -5043,7 +4952,7 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -5053,7 +4962,7 @@
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
@@ -5063,7 +4972,7 @@
     </row>
     <row r="6" spans="1:703" ht="23" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -5073,7 +4982,7 @@
     </row>
     <row r="7" spans="1:703" ht="23" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
@@ -5083,7 +4992,7 @@
     </row>
     <row r="8" spans="1:703" ht="23" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
@@ -5093,340 +5002,380 @@
     </row>
     <row r="9" spans="1:703" ht="23" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>268</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="HA9" s="6"/>
       <c r="AAA9" s="6"/>
     </row>
     <row r="10" spans="1:703" ht="23" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="HA10" s="6"/>
       <c r="AAA10" s="6"/>
     </row>
     <row r="11" spans="1:703" ht="23" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>196</v>
+        <v>276</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="HA11" s="6"/>
       <c r="AAA11" s="6"/>
     </row>
     <row r="12" spans="1:703" ht="23" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>197</v>
+        <v>277</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>198</v>
+        <v>257</v>
       </c>
       <c r="HA12" s="6"/>
       <c r="AAA12" s="6"/>
     </row>
     <row r="13" spans="1:703" ht="23" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>199</v>
+        <v>271</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>200</v>
+        <v>272</v>
       </c>
       <c r="HA13" s="6"/>
       <c r="AAA13" s="6"/>
     </row>
     <row r="14" spans="1:703" ht="23" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="HA14" s="4"/>
-      <c r="AAA14" s="5"/>
+        <v>195</v>
+      </c>
+      <c r="HA14" s="6"/>
+      <c r="AAA14" s="6"/>
     </row>
     <row r="15" spans="1:703" ht="23" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="HA15" s="4"/>
-      <c r="AAA15" s="5"/>
+        <v>198</v>
+      </c>
+      <c r="HA15" s="6"/>
+      <c r="AAA15" s="6"/>
     </row>
     <row r="16" spans="1:703" ht="23" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="HA16" s="4"/>
-      <c r="AAA16" s="5"/>
+        <v>200</v>
+      </c>
+      <c r="HA16" s="6"/>
+      <c r="AAA16" s="6"/>
     </row>
     <row r="17" spans="1:703" ht="23" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="HA17" s="4"/>
       <c r="AAA17" s="5"/>
     </row>
     <row r="18" spans="1:703" ht="23" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="HA18" s="4"/>
       <c r="AAA18" s="5"/>
     </row>
     <row r="19" spans="1:703" ht="23" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="HA19" s="4"/>
       <c r="AAA19" s="5"/>
     </row>
     <row r="20" spans="1:703" ht="23" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="HA20" s="4"/>
       <c r="AAA20" s="5"/>
     </row>
     <row r="21" spans="1:703" ht="23" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="HA21" s="4"/>
       <c r="AAA21" s="5"/>
     </row>
     <row r="22" spans="1:703" ht="23" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>218</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="HA22" s="4"/>
+      <c r="AAA22" s="5"/>
     </row>
     <row r="23" spans="1:703" ht="23" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>220</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="HA23" s="4"/>
+      <c r="AAA23" s="5"/>
     </row>
     <row r="24" spans="1:703" ht="23" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>249</v>
+        <v>212</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>248</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="HA24" s="4"/>
+      <c r="AAA24" s="5"/>
     </row>
     <row r="25" spans="1:703" ht="23" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>221</v>
+        <v>273</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>235</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="HA25" s="4"/>
+      <c r="AAA25" s="5"/>
     </row>
     <row r="26" spans="1:703" ht="23" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:703" ht="23" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:703" ht="23" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>228</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:703" ht="23" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>225</v>
+        <v>275</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>229</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:703" ht="23" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:703" ht="23" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>231</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:703" ht="23" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>263</v>
+        <v>222</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>264</v>
+        <v>235</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="23" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="23" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>267</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="23" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="23" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="23" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>239</v>
+        <v>262</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>240</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="23" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>244</v>
+        <v>265</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>245</v>
+        <v>264</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="23" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="23" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="23" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="23" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>119</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="23" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="23" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>11</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="23" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="23" customHeight="1">
+      <c r="A46" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="23" customHeight="1">
+      <c r="A47" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="23" customHeight="1">
+      <c r="A48" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="23" customHeight="1">
+      <c r="A49" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="23" customHeight="1">
+      <c r="A50" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="23" customHeight="1">
+      <c r="A51" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -5434,88 +5383,88 @@
   <sortState ref="A1:B6">
     <sortCondition ref="A1:A6"/>
   </sortState>
-  <conditionalFormatting sqref="A29:A41 A46:A1048576 A25:A26">
+  <conditionalFormatting sqref="A34:A47 A52:A1048576 A30:A31">
     <cfRule type="beginsWith" dxfId="44" priority="49" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A30,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="43" priority="50" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A30,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="42" priority="51" stopIfTrue="1">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B29:B41 B46:B1048576 B24:B26">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:B47 B52:B1048576 B28:B31">
     <cfRule type="expression" dxfId="41" priority="52" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="40" priority="53">
-      <formula>LEN(TRIM(B24))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11:A19 A21:A24">
+      <formula>LEN(TRIM(B28))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:A22 A24:A29">
     <cfRule type="beginsWith" dxfId="39" priority="44" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A11,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="38" priority="45" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A11,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="37" priority="46" stopIfTrue="1">
-      <formula>LEN(TRIM(A11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B19 B21:B22 B24">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:B22 B24:B26 B28:B29">
     <cfRule type="expression" dxfId="36" priority="47" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="35" priority="48">
-      <formula>LEN(TRIM(B11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
+      <formula>LEN(TRIM(B14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
     <cfRule type="beginsWith" dxfId="34" priority="36" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A20,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="33" priority="37" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A20,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="32" priority="38" stopIfTrue="1">
-      <formula>LEN(TRIM(A20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23">
     <cfRule type="expression" dxfId="31" priority="39" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="30" priority="40">
-      <formula>LEN(TRIM(B20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
+      <formula>LEN(TRIM(B23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
     <cfRule type="expression" dxfId="29" priority="34" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="28" priority="35">
-      <formula>LEN(TRIM(B23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27:A28">
+      <formula>LEN(TRIM(B27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32:A33">
     <cfRule type="beginsWith" dxfId="27" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A32,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="26" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A32,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="25" priority="31" stopIfTrue="1">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27:B28">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:B33">
     <cfRule type="expression" dxfId="24" priority="32" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="23" priority="33">
-      <formula>LEN(TRIM(B27))&gt;0</formula>
+      <formula>LEN(TRIM(B32))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A4">
@@ -5537,7 +5486,7 @@
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A10">
+  <conditionalFormatting sqref="A5:A13">
     <cfRule type="beginsWith" dxfId="17" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A5,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
@@ -5548,7 +5497,7 @@
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B10">
+  <conditionalFormatting sqref="B5:B13">
     <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
@@ -5556,53 +5505,53 @@
       <formula>LEN(TRIM(B5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A44:A45">
+  <conditionalFormatting sqref="A50:A51">
     <cfRule type="beginsWith" dxfId="12" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A44,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A50,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="11" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A44,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A50,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="10" priority="11" stopIfTrue="1">
-      <formula>LEN(TRIM(A44))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B42:B43 B45">
+      <formula>LEN(TRIM(A50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48:B49 B51">
     <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="8" priority="13">
-      <formula>LEN(TRIM(B42))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
+      <formula>LEN(TRIM(B48))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
     <cfRule type="beginsWith" dxfId="7" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A42,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A48,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="6" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A42,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A48,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="6" stopIfTrue="1">
-      <formula>LEN(TRIM(A42))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B42">
+      <formula>LEN(TRIM(A48))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48">
     <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="3" priority="8">
-      <formula>LEN(TRIM(B42))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43">
+      <formula>LEN(TRIM(B48))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
     <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A43,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A49,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A43,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A49,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(A43))&gt;0</formula>
+      <formula>LEN(TRIM(A49))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[General] - support specifying data variable override via command line. Same effect as using `set JAVA_OPT=-D...` but this may be   simpler for some folks.
[Built-in Function]
- support for `informal` date/time formatting to mimic human conversation.

[Nexial Expression]
- [DATE expression](../expressions/DATEexpression): support for `informal` date/time formatting to mimic human
  conversation.

[web]
- [`focus(locator)`](../commands/web/focus(locator)): **NEW** command to place cursor focus on the first element that
  matches specified `locator`. Note that if the matched element is a textbox or textarea, Nexial will also automate a
  click to put the cursor on the target INPUT element.
- code enhanced to stabilize webdriver initialization between different browsers.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-03.data.xlsx
+++ b/artifact/data/web-03.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE980A37-8077-9B4E-8621-A83C5AF60558}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58F73BB-AFBF-F045-8B13-EED8F1F89FDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="15780" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="10520" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="292">
   <si>
     <t>true</t>
   </si>
@@ -797,9 +797,6 @@
     <t>deal.output.file</t>
   </si>
   <si>
-    <t>$(syspath|out|fullpath)/mydeals.html</t>
-  </si>
-  <si>
     <t>deal.item.template</t>
   </si>
   <si>
@@ -872,9 +869,6 @@
     <t>//nexial.enforcePageSourceStability</t>
   </si>
   <si>
-    <t>//nexial.web.alwaysWait</t>
-  </si>
-  <si>
     <t>TABLET|TV|ECHO|PHONE|GEAR|TOY|GAME|MUSIC|LAPTOP|SPEAKER|CABLE|SAMSUNG|MONITOR|WIRE|USB|MOUNT|HD</t>
   </si>
   <si>
@@ -911,10 +905,40 @@
     <t>//div[@id='FilterItemView_all_summary' and contains(normalize-space(string(.)), '${desired availability type} : ${desired review stars} Stars &amp; Up')]</t>
   </si>
   <si>
-    <t>300</t>
-  </si>
-  <si>
     <t>5000</t>
+  </si>
+  <si>
+    <t>chrome.headless</t>
+  </si>
+  <si>
+    <t>firefox.headless</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>safari</t>
+  </si>
+  <si>
+    <t>1-5</t>
+  </si>
+  <si>
+    <t>800</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>nexial.web.alwaysWait</t>
+  </si>
+  <si>
+    <t>deal.output.base</t>
+  </si>
+  <si>
+    <t>$(syspath|out|fullpath)/${nexial.browser}</t>
+  </si>
+  <si>
+    <t>${deal.output.base}/mydeals.html</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1081,44 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="145">
+  <dxfs count="148">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -3225,7 +3286,7 @@
   <dimension ref="A1:AAA21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B9" sqref="A9:B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -3378,40 +3439,40 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1 A3:A9 A22:A1048576">
-    <cfRule type="beginsWith" dxfId="144" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="147" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="143" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="146" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="142" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="145" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1 B3:B9 B22:B1048576">
-    <cfRule type="expression" dxfId="141" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="140" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="143" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="beginsWith" dxfId="139" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="142" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="138" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="141" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="137" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="140" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="136" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="135" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="138" priority="5">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3529,21 +3590,21 @@
     <sortCondition ref="A1:A9"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="134" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="137" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="133" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="136" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="132" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="135" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="131" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="130" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="133" priority="12">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3630,40 +3691,40 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="129" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="132" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="128" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="131" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="127" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="130" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="126" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="125" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="128" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A12">
-    <cfRule type="beginsWith" dxfId="124" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="127" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="123" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="126" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="122" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="125" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B12">
-    <cfRule type="expression" dxfId="121" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="120" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="123" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3752,32 +3813,32 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="beginsWith" dxfId="119" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="122" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="118" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="121" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="117" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="120" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="116" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="115" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="118" priority="13">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="beginsWith" dxfId="114" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="117" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="113" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="116" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="112" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="115" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4029,130 +4090,130 @@
     <sortCondition ref="A17:A25"/>
   </sortState>
   <conditionalFormatting sqref="A18:A20 A22 A26:A1048576 A1:A13">
-    <cfRule type="beginsWith" dxfId="111" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="114" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="110" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="113" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="109" priority="42" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="112" priority="42" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 B10:B13 B22 B26:B1048576 B1:B8">
-    <cfRule type="expression" dxfId="108" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="43" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="107" priority="44">
+    <cfRule type="notContainsBlanks" dxfId="110" priority="44">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="106" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="109" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="105" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="108" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="104" priority="34" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="107" priority="34" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="beginsWith" dxfId="103" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="106" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="102" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="105" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="101" priority="31" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="104" priority="31" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:A17">
-    <cfRule type="beginsWith" dxfId="100" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="103" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="99" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="102" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="98" priority="28" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="101" priority="28" stopIfTrue="1">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="beginsWith" dxfId="97" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="100" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A21,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="96" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="99" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A21,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="95" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="98" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="94" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="93" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="96" priority="20">
       <formula>LEN(TRIM(B21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="beginsWith" dxfId="92" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="95" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="91" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="94" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="90" priority="13" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="93" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="89" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="88" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="91" priority="15">
       <formula>LEN(TRIM(B23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="beginsWith" dxfId="87" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="90" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="86" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="89" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="85" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="88" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="84" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="83" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="86" priority="10">
       <formula>LEN(TRIM(B25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="beginsWith" dxfId="82" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="85" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A24,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="81" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="84" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A24,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="80" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="79" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="78" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="81" priority="5">
       <formula>LEN(TRIM(B24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4336,59 +4397,59 @@
     <sortCondition ref="A1:A15"/>
   </sortState>
   <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="77" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="80" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="76" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="79" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="75" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="74" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="73" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="76" priority="18">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="beginsWith" dxfId="72" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="75" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A11,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="71" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="74" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A11,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="70" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="expression" dxfId="69" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="68" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="13">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A10">
-    <cfRule type="beginsWith" dxfId="67" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="70" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="66" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="69" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="65" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B10">
-    <cfRule type="expression" dxfId="64" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="63" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4581,21 +4642,21 @@
     <sortCondition ref="A1:A16"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="62" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="65" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="61" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="64" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="60" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="59" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="58" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4850,51 +4911,51 @@
     <sortCondition ref="A1:A25"/>
   </sortState>
   <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="beginsWith" dxfId="57" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="60" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="56" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="59" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="55" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B1048576 B13:B14">
-    <cfRule type="expression" dxfId="54" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="53" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="13">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="beginsWith" dxfId="52" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="55" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="51" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="54" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="50" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B13">
-    <cfRule type="expression" dxfId="49" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="48" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="47" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="50" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="49" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="45" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4905,64 +4966,76 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15D721F-E928-8949-A67C-84C364E740E7}">
-  <dimension ref="A1:AAA51"/>
+  <dimension ref="A1:AAA53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="34.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="103.1640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="94.33203125" style="2" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:703" ht="23" customHeight="1">
+    <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>242</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>285</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703" ht="23" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>256</v>
+        <v>2</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703" ht="23" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>254</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>255</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>284</v>
       </c>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>254</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="HA4" s="6"/>
       <c r="AAA4" s="6"/>
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
@@ -4972,7 +5045,7 @@
     </row>
     <row r="6" spans="1:703" ht="23" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -4982,7 +5055,7 @@
     </row>
     <row r="7" spans="1:703" ht="23" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
@@ -4992,569 +5065,607 @@
     </row>
     <row r="8" spans="1:703" ht="23" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="HA8" s="6"/>
       <c r="AAA8" s="6"/>
     </row>
     <row r="9" spans="1:703" ht="23" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>267</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>282</v>
+        <v>0</v>
       </c>
       <c r="HA9" s="6"/>
       <c r="AAA9" s="6"/>
     </row>
     <row r="10" spans="1:703" ht="23" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>267</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>283</v>
+        <v>194</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>286</v>
       </c>
       <c r="HA10" s="6"/>
       <c r="AAA10" s="6"/>
     </row>
     <row r="11" spans="1:703" ht="23" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>0</v>
+        <v>280</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>287</v>
       </c>
       <c r="HA11" s="6"/>
       <c r="AAA11" s="6"/>
     </row>
     <row r="12" spans="1:703" ht="23" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="HA12" s="6"/>
       <c r="AAA12" s="6"/>
     </row>
     <row r="13" spans="1:703" ht="23" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="HA13" s="6"/>
       <c r="AAA13" s="6"/>
     </row>
     <row r="14" spans="1:703" ht="23" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>196</v>
+        <v>269</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>195</v>
+        <v>270</v>
       </c>
       <c r="HA14" s="6"/>
       <c r="AAA14" s="6"/>
     </row>
     <row r="15" spans="1:703" ht="23" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="HA15" s="6"/>
       <c r="AAA15" s="6"/>
     </row>
     <row r="16" spans="1:703" ht="23" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="HA16" s="6"/>
       <c r="AAA16" s="6"/>
     </row>
     <row r="17" spans="1:703" ht="23" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="HA17" s="4"/>
-      <c r="AAA17" s="5"/>
+        <v>200</v>
+      </c>
+      <c r="HA17" s="6"/>
+      <c r="AAA17" s="6"/>
     </row>
     <row r="18" spans="1:703" ht="23" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="HA18" s="4"/>
       <c r="AAA18" s="5"/>
     </row>
     <row r="19" spans="1:703" ht="23" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="HA19" s="4"/>
       <c r="AAA19" s="5"/>
     </row>
     <row r="20" spans="1:703" ht="23" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="HA20" s="4"/>
       <c r="AAA20" s="5"/>
     </row>
     <row r="21" spans="1:703" ht="23" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="HA21" s="4"/>
       <c r="AAA21" s="5"/>
     </row>
     <row r="22" spans="1:703" ht="23" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="HA22" s="4"/>
       <c r="AAA22" s="5"/>
     </row>
     <row r="23" spans="1:703" ht="23" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="HA23" s="4"/>
       <c r="AAA23" s="5"/>
     </row>
     <row r="24" spans="1:703" ht="23" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="HA24" s="4"/>
       <c r="AAA24" s="5"/>
     </row>
     <row r="25" spans="1:703" ht="23" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>273</v>
+        <v>212</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>274</v>
+        <v>217</v>
       </c>
       <c r="HA25" s="4"/>
       <c r="AAA25" s="5"/>
     </row>
     <row r="26" spans="1:703" ht="23" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>214</v>
+        <v>271</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>280</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="HA26" s="4"/>
+      <c r="AAA26" s="5"/>
     </row>
     <row r="27" spans="1:703" ht="23" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>219</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:703" ht="23" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>248</v>
+        <v>218</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:703" ht="23" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
     </row>
     <row r="30" spans="1:703" ht="23" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>220</v>
+        <v>273</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>234</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:703" ht="23" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:703" ht="23" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>235</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="23" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="23" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="23" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="23" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="23" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>263</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="23" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="23" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>231</v>
+        <v>264</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="23" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>233</v>
+        <v>265</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="23" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="23" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="23" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="23" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>245</v>
+        <v>289</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>259</v>
+        <v>290</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="23" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>250</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="23" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="23" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>278</v>
+        <v>248</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>279</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="23" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>119</v>
+        <v>251</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="23" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="23" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>11</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="23" customHeight="1">
       <c r="A51" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="23" customHeight="1">
+      <c r="A52" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="23" customHeight="1">
+      <c r="A53" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>194</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <sortState ref="A1:B6">
-    <sortCondition ref="A1:A6"/>
+  <sortState ref="A2:B7">
+    <sortCondition ref="A2:A7"/>
   </sortState>
-  <conditionalFormatting sqref="A34:A47 A52:A1048576 A30:A31">
-    <cfRule type="beginsWith" dxfId="44" priority="49" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A30,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="43" priority="50" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A30,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="42" priority="51" stopIfTrue="1">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B34:B47 B52:B1048576 B28:B31">
-    <cfRule type="expression" dxfId="41" priority="52" stopIfTrue="1">
+  <conditionalFormatting sqref="A35:A49 A54:A1048576 A31:A32">
+    <cfRule type="beginsWith" dxfId="47" priority="55" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A31,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="46" priority="56" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A31,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="45" priority="57" stopIfTrue="1">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54:B1048576 B29:B32 B35:B49">
+    <cfRule type="expression" dxfId="44" priority="58" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="40" priority="53">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="59">
+      <formula>LEN(TRIM(B29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:A23 A25:A30">
+    <cfRule type="beginsWith" dxfId="42" priority="50" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="41" priority="51" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="40" priority="52" stopIfTrue="1">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:B23 B25:B27 B29:B30">
+    <cfRule type="expression" dxfId="39" priority="53" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="38" priority="54">
+      <formula>LEN(TRIM(B15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="beginsWith" dxfId="37" priority="42" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A24,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="36" priority="43" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A24,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="35" priority="44" stopIfTrue="1">
+      <formula>LEN(TRIM(A24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="expression" dxfId="34" priority="45" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="33" priority="46">
+      <formula>LEN(TRIM(B24))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
+    <cfRule type="expression" dxfId="32" priority="40" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="31" priority="41">
       <formula>LEN(TRIM(B28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:A22 A24:A29">
-    <cfRule type="beginsWith" dxfId="39" priority="44" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="38" priority="45" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="37" priority="46" stopIfTrue="1">
-      <formula>LEN(TRIM(A14))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:B22 B24:B26 B28:B29">
-    <cfRule type="expression" dxfId="36" priority="47" stopIfTrue="1">
+  <conditionalFormatting sqref="A33:A34">
+    <cfRule type="beginsWith" dxfId="30" priority="35" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A33,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="29" priority="36" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A33,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="28" priority="37" stopIfTrue="1">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33:B34">
+    <cfRule type="expression" dxfId="27" priority="38" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="35" priority="48">
-      <formula>LEN(TRIM(B14))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="beginsWith" dxfId="34" priority="36" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="33" priority="37" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="32" priority="38" stopIfTrue="1">
-      <formula>LEN(TRIM(A23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="31" priority="39" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="39">
+      <formula>LEN(TRIM(B33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A5">
+    <cfRule type="beginsWith" dxfId="25" priority="25" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="24" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="23" priority="27" stopIfTrue="1">
+      <formula>LEN(TRIM(A2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B5">
+    <cfRule type="expression" dxfId="22" priority="28" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="30" priority="40">
-      <formula>LEN(TRIM(B23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="29" priority="34" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="29">
+      <formula>LEN(TRIM(B2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:A14">
+    <cfRule type="beginsWith" dxfId="20" priority="20" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A6,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="19" priority="21" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A6,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="18" priority="22" stopIfTrue="1">
+      <formula>LEN(TRIM(A6))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:B14">
+    <cfRule type="expression" dxfId="17" priority="23" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="28" priority="35">
-      <formula>LEN(TRIM(B27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32:A33">
-    <cfRule type="beginsWith" dxfId="27" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A32,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A32,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="25" priority="31" stopIfTrue="1">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B32:B33">
-    <cfRule type="expression" dxfId="24" priority="32" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="24">
+      <formula>LEN(TRIM(B6))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52:A53">
+    <cfRule type="beginsWith" dxfId="15" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A52,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="14" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A52,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="13" priority="17" stopIfTrue="1">
+      <formula>LEN(TRIM(A52))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50:B51 B53">
+    <cfRule type="expression" dxfId="12" priority="18" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="23" priority="33">
-      <formula>LEN(TRIM(B32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A4">
-    <cfRule type="beginsWith" dxfId="22" priority="19" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="19">
+      <formula>LEN(TRIM(B50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="beginsWith" dxfId="10" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A50,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="9" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A50,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="8" priority="12" stopIfTrue="1">
+      <formula>LEN(TRIM(A50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50">
+    <cfRule type="expression" dxfId="7" priority="13" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="6" priority="14">
+      <formula>LEN(TRIM(B50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="beginsWith" dxfId="5" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A51,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="4" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A51,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="9" stopIfTrue="1">
+      <formula>LEN(TRIM(A51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="21" priority="20" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="20" priority="21" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B4">
-    <cfRule type="expression" dxfId="19" priority="22" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="23">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A13">
-    <cfRule type="beginsWith" dxfId="17" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A5,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A5,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="15" priority="16" stopIfTrue="1">
-      <formula>LEN(TRIM(A5))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B13">
-    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="13" priority="18">
-      <formula>LEN(TRIM(B5))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50:A51">
-    <cfRule type="beginsWith" dxfId="12" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A50,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="11" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A50,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11" stopIfTrue="1">
-      <formula>LEN(TRIM(A50))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B48:B49 B51">
-    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="8" priority="13">
-      <formula>LEN(TRIM(B48))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
-    <cfRule type="beginsWith" dxfId="7" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A48,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A48,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6" stopIfTrue="1">
-      <formula>LEN(TRIM(A48))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="8">
-      <formula>LEN(TRIM(B48))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A49,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A49,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(A49))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="B13 B22 B50 B52:B53" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[web] - [web &raquo; `typeKeys(locator,value)`](../commands/web/typeKeys(locator,value)): automatically adds `TAB` when   `value` is `(empty)` so that the appropriate HTML event may be triggered. - prevent the evaluation of fail-fast when command does not result in a FAIL condition (e.g. SKIP)
- added more references to web documentation
- tutorial: web-03 now completes with Amazon example (one in XPATH, the other CSS)
- add comments/docs to WebCommand.java

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-03.data.xlsx
+++ b/artifact/data/web-03.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58F73BB-AFBF-F045-8B13-EED8F1F89FDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8446527-20CE-8E41-BD2E-066E4805A82D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="10520" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="15780" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -21,10 +21,11 @@
     <sheet name="locators-name" sheetId="7" r:id="rId6"/>
     <sheet name="locators-css" sheetId="4" r:id="rId7"/>
     <sheet name="locators-xpath" sheetId="8" r:id="rId8"/>
-    <sheet name="locators-xpath2" sheetId="10" r:id="rId9"/>
+    <sheet name="locators-amazon1" sheetId="10" r:id="rId9"/>
+    <sheet name="locators-amazon2" sheetId="11" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="313">
   <si>
     <t>true</t>
   </si>
@@ -833,9 +834,6 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
     <t>desired product keywords</t>
   </si>
   <si>
@@ -866,9 +864,6 @@
     <t>nexial.web.pageLoadWaitMs</t>
   </si>
   <si>
-    <t>//nexial.enforcePageSourceStability</t>
-  </si>
-  <si>
     <t>TABLET|TV|ECHO|PHONE|GEAR|TOY|GAME|MUSIC|LAPTOP|SPEAKER|CABLE|SAMSUNG|MONITOR|WIRE|USB|MOUNT|HD</t>
   </si>
   <si>
@@ -905,9 +900,6 @@
     <t>//div[@id='FilterItemView_all_summary' and contains(normalize-space(string(.)), '${desired availability type} : ${desired review stars} Stars &amp; Up')]</t>
   </si>
   <si>
-    <t>5000</t>
-  </si>
-  <si>
     <t>chrome.headless</t>
   </si>
   <si>
@@ -926,12 +918,6 @@
     <t>800</t>
   </si>
   <si>
-    <t>10000</t>
-  </si>
-  <si>
-    <t>nexial.web.alwaysWait</t>
-  </si>
-  <si>
     <t>deal.output.base</t>
   </si>
   <si>
@@ -939,13 +925,433 @@
   </si>
   <si>
     <t>${deal.output.base}/mydeals.html</t>
+  </si>
+  <si>
+    <t>browser comparison csv</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/web-03-browser-comparison.csv</t>
+  </si>
+  <si>
+    <t>nexial.failAfter</t>
+  </si>
+  <si>
+    <t>4500</t>
+  </si>
+  <si>
+    <t>9000</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>class=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>gbh1-bold</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>css=</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>div#navFooter &gt; a[href='#nav-top'] span.navFooterBackToTopText</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>id=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>widgetFilters</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>xpath=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>//*[@id='widgetFilters']//div[./*[normalize-space(text())="Availability"]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>xpath=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>//*[@id='widgetFilters']//div[./*[normalize-space(text())="Avg. Customer Review"]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>css=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>.widgetContainer #widgetContent .tallCellView</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>xpath=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>//table[contains(@class, "navFooterMoreOnAmazon")]//td[contains(@class,"navFooterDescItem")]/a[starts-with(text(),"Amazon")]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>css=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>div[id='${deal.item.id}']</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>css=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>div[id='${deal.item.id}'] .priceBlock &gt; span</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>css=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>div[id='${deal.item.id}'] #${deal.item.id}_dealClock</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>css=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>div[id='${deal.item.id}'] #dealTitle</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>css=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>div[id='${deal.item.id}'] #shipSoldInfo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>css=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>div[id='${deal.item.id}'] .reviewStars .a-color-base</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>css=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>div[id='${deal.item.id}'] .stackToBottom button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>css=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>div[id='${deal.item.id}'] .stackToBottom</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>xpath=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>//div[@id='FilterItemView_page_pagination']//span[@class='a-declarative']/div[not(contains(@class,'hidden'))]/*[contains(@class,'a-pagination')]/*[@class='a-last']/a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>css=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>#FilterItemView_all_summary &gt; div</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>css=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>div[id='${deal.item.id}'] a#dealImage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>css=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>div[id='${deal.item.id}'] a#dealImage img</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>xpath=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>//div[@id='FilterItemView_all_summary' and contains(normalize-space(string(.)), '${desired availability type} : ${desired review stars} Stars &amp; Up')]</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -994,6 +1400,21 @@
     <font>
       <i/>
       <sz val="12"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="5"/>
       <name val="Courier New"/>
       <family val="1"/>
     </font>
@@ -1081,81 +1502,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="148">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="188">
     <dxf>
       <font>
         <b val="0"/>
@@ -1181,6 +1528,600 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3439,41 +4380,729 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1 A3:A9 A22:A1048576">
-    <cfRule type="beginsWith" dxfId="147" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="187" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="146" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="186" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="145" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="185" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1 B3:B9 B22:B1048576">
-    <cfRule type="expression" dxfId="144" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="184" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="143" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="183" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="beginsWith" dxfId="142" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="182" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="141" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="181" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="140" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="180" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="139" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="179" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="138" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="178" priority="5">
       <formula>LEN(TRIM(B2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03856218-1A13-8840-A44A-29262810A7AA}">
+  <dimension ref="A1:AAA53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="34.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="94.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703" ht="23" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703" ht="23" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
+    </row>
+    <row r="4" spans="1:703" ht="23" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="HA4" s="6"/>
+      <c r="AAA4" s="6"/>
+    </row>
+    <row r="5" spans="1:703" ht="23" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="HA5" s="6"/>
+      <c r="AAA5" s="6"/>
+    </row>
+    <row r="6" spans="1:703" ht="23" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="HA6" s="6"/>
+      <c r="AAA6" s="6"/>
+    </row>
+    <row r="7" spans="1:703" ht="23" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="HA7" s="6"/>
+      <c r="AAA7" s="6"/>
+    </row>
+    <row r="8" spans="1:703" ht="23" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="HA8" s="6"/>
+      <c r="AAA8" s="6"/>
+    </row>
+    <row r="9" spans="1:703" ht="23" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="HA9" s="6"/>
+      <c r="AAA9" s="6"/>
+    </row>
+    <row r="10" spans="1:703" ht="23" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="HA10" s="6"/>
+      <c r="AAA10" s="6"/>
+    </row>
+    <row r="11" spans="1:703" ht="23" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="HA11" s="6"/>
+      <c r="AAA11" s="6"/>
+    </row>
+    <row r="12" spans="1:703" ht="23" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="HA12" s="6"/>
+      <c r="AAA12" s="6"/>
+    </row>
+    <row r="13" spans="1:703" ht="23" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="HA13" s="6"/>
+      <c r="AAA13" s="6"/>
+    </row>
+    <row r="14" spans="1:703" ht="23" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="HA14" s="6"/>
+      <c r="AAA14" s="6"/>
+    </row>
+    <row r="15" spans="1:703" ht="23" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="HA15" s="6"/>
+      <c r="AAA15" s="6"/>
+    </row>
+    <row r="16" spans="1:703" ht="23" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="HA16" s="6"/>
+      <c r="AAA16" s="6"/>
+    </row>
+    <row r="17" spans="1:703" ht="23" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="HA17" s="4"/>
+      <c r="AAA17" s="5"/>
+    </row>
+    <row r="18" spans="1:703" ht="23" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="HA18" s="4"/>
+      <c r="AAA18" s="5"/>
+    </row>
+    <row r="19" spans="1:703" ht="23" customHeight="1">
+      <c r="A19" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="HA19" s="4"/>
+      <c r="AAA19" s="5"/>
+    </row>
+    <row r="20" spans="1:703" ht="23" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="HA20" s="4"/>
+      <c r="AAA20" s="5"/>
+    </row>
+    <row r="21" spans="1:703" ht="23" customHeight="1">
+      <c r="A21" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="HA21" s="4"/>
+      <c r="AAA21" s="5"/>
+    </row>
+    <row r="22" spans="1:703" ht="23" customHeight="1">
+      <c r="A22" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="HA22" s="4"/>
+      <c r="AAA22" s="5"/>
+    </row>
+    <row r="23" spans="1:703" ht="23" customHeight="1">
+      <c r="A23" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="HA23" s="4"/>
+      <c r="AAA23" s="5"/>
+    </row>
+    <row r="24" spans="1:703" ht="23" customHeight="1">
+      <c r="A24" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="HA24" s="4"/>
+      <c r="AAA24" s="5"/>
+    </row>
+    <row r="25" spans="1:703" ht="23" customHeight="1">
+      <c r="A25" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="HA25" s="4"/>
+      <c r="AAA25" s="5"/>
+    </row>
+    <row r="26" spans="1:703" ht="23" customHeight="1">
+      <c r="A26" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="27" spans="1:703" ht="23" customHeight="1">
+      <c r="A27" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="28" spans="1:703" ht="23" customHeight="1">
+      <c r="A28" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="29" spans="1:703" ht="23" customHeight="1">
+      <c r="A29" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="30" spans="1:703" ht="23" customHeight="1">
+      <c r="A30" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="31" spans="1:703" ht="23" customHeight="1">
+      <c r="A31" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:703" ht="23" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" ht="23" customHeight="1">
+      <c r="A33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="23" customHeight="1">
+      <c r="A34" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="23" customHeight="1">
+      <c r="A35" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="23" customHeight="1">
+      <c r="A36" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="23" customHeight="1">
+      <c r="A37" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="23" customHeight="1">
+      <c r="A38" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="23" customHeight="1">
+      <c r="A39" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="23" customHeight="1">
+      <c r="A40" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="23" customHeight="1">
+      <c r="A41" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="23" customHeight="1">
+      <c r="A42" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="23" customHeight="1">
+      <c r="A43" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="23" customHeight="1">
+      <c r="A44" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="23" customHeight="1">
+      <c r="A45" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="23" customHeight="1">
+      <c r="A46" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="23" customHeight="1">
+      <c r="A47" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="23" customHeight="1">
+      <c r="A48" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="23" customHeight="1">
+      <c r="A49" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="23" customHeight="1">
+      <c r="A50" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="23" customHeight="1">
+      <c r="A51" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="23" customHeight="1">
+      <c r="A52" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="23" customHeight="1">
+      <c r="A53" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A34:A49 A54:A1048576 A30:A31 A7:A13">
+    <cfRule type="beginsWith" dxfId="44" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A7,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="43" priority="42" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A7,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="42" priority="43" stopIfTrue="1">
+      <formula>LEN(TRIM(A7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54:B1048576 B28:B31 B34:B49 B7:B13">
+    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="40" priority="45">
+      <formula>LEN(TRIM(B7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:A22 A24:A29">
+    <cfRule type="beginsWith" dxfId="39" priority="36" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="38" priority="37" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="37" priority="38" stopIfTrue="1">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:B22 B24:B26 B28:B29">
+    <cfRule type="expression" dxfId="36" priority="39" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="35" priority="40">
+      <formula>LEN(TRIM(B14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="beginsWith" dxfId="34" priority="31" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="33" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="32" priority="33" stopIfTrue="1">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23">
+    <cfRule type="expression" dxfId="31" priority="34" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="30" priority="35">
+      <formula>LEN(TRIM(B23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="expression" dxfId="29" priority="29" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="28" priority="30">
+      <formula>LEN(TRIM(B27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32:A33">
+    <cfRule type="beginsWith" dxfId="27" priority="24" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A32,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="26" priority="25" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A32,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="25" priority="26" stopIfTrue="1">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:B33">
+    <cfRule type="expression" dxfId="24" priority="27" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="23" priority="28">
+      <formula>LEN(TRIM(B32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A6">
+    <cfRule type="beginsWith" dxfId="22" priority="19" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="21" priority="20" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="20" priority="21" stopIfTrue="1">
+      <formula>LEN(TRIM(A2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B6">
+    <cfRule type="expression" dxfId="19" priority="22" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="18" priority="23">
+      <formula>LEN(TRIM(B2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52:A53">
+    <cfRule type="beginsWith" dxfId="17" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A52,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="16" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A52,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="15" priority="16" stopIfTrue="1">
+      <formula>LEN(TRIM(A52))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50:B51 B53">
+    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="13" priority="18">
+      <formula>LEN(TRIM(B50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="beginsWith" dxfId="12" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A50,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="11" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A50,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11" stopIfTrue="1">
+      <formula>LEN(TRIM(A50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50">
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="8" priority="13">
+      <formula>LEN(TRIM(B50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="beginsWith" dxfId="7" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A51,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="6" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A51,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="beginsWith" dxfId="4" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="2" priority="5" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
+      <formula>LEN(TRIM(C32))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3590,21 +5219,21 @@
     <sortCondition ref="A1:A9"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="137" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="177" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="136" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="176" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="135" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="175" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="134" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="174" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="133" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="173" priority="12">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3691,40 +5320,40 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="132" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="172" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="131" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="171" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="130" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="170" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="129" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="169" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="128" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="168" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A12">
-    <cfRule type="beginsWith" dxfId="127" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="167" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="126" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="166" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="125" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="165" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B12">
-    <cfRule type="expression" dxfId="124" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="164" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="123" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="163" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3813,32 +5442,32 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="beginsWith" dxfId="122" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="162" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="121" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="161" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="120" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="160" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="119" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="118" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="158" priority="13">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="beginsWith" dxfId="117" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="157" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="116" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="156" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="115" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="155" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4090,130 +5719,130 @@
     <sortCondition ref="A17:A25"/>
   </sortState>
   <conditionalFormatting sqref="A18:A20 A22 A26:A1048576 A1:A13">
-    <cfRule type="beginsWith" dxfId="114" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="154" priority="40" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="113" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="153" priority="41" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="112" priority="42" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="152" priority="42" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 B10:B13 B22 B26:B1048576 B1:B8">
-    <cfRule type="expression" dxfId="111" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="43" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="110" priority="44">
+    <cfRule type="notContainsBlanks" dxfId="150" priority="44">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="109" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="149" priority="32" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="108" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="148" priority="33" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="107" priority="34" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="147" priority="34" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="beginsWith" dxfId="106" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="146" priority="29" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="105" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="145" priority="30" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="104" priority="31" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="144" priority="31" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:A17">
-    <cfRule type="beginsWith" dxfId="103" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="143" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="102" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="142" priority="27" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="101" priority="28" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="141" priority="28" stopIfTrue="1">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="beginsWith" dxfId="100" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="140" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A21,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="99" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="139" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A21,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="98" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="138" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="97" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="96" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="136" priority="20">
       <formula>LEN(TRIM(B21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="beginsWith" dxfId="95" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="135" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="94" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="134" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="93" priority="13" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="133" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="92" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="91" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="131" priority="15">
       <formula>LEN(TRIM(B23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="beginsWith" dxfId="90" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="130" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="89" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="129" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="88" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="128" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="87" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="86" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="126" priority="10">
       <formula>LEN(TRIM(B25))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="beginsWith" dxfId="85" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="125" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A24,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="84" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="124" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A24,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="83" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="123" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="82" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="81" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="121" priority="5">
       <formula>LEN(TRIM(B24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4397,59 +6026,59 @@
     <sortCondition ref="A1:A15"/>
   </sortState>
   <conditionalFormatting sqref="A13:A1048576">
-    <cfRule type="beginsWith" dxfId="80" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="120" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="79" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="119" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="78" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="118" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576">
-    <cfRule type="expression" dxfId="77" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="76" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="116" priority="18">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="beginsWith" dxfId="75" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="115" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A11,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="74" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="114" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A11,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="73" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="113" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="expression" dxfId="72" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="71" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="111" priority="13">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A10">
-    <cfRule type="beginsWith" dxfId="70" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="110" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="69" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="109" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="68" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="108" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B10">
-    <cfRule type="expression" dxfId="67" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="66" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="106" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4642,21 +6271,21 @@
     <sortCondition ref="A1:A16"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="65" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="105" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="64" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="104" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="63" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="103" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="62" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="61" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="101" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4911,51 +6540,51 @@
     <sortCondition ref="A1:A25"/>
   </sortState>
   <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="beginsWith" dxfId="60" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="100" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="59" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="99" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="58" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="98" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B1048576 B13:B14">
-    <cfRule type="expression" dxfId="57" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="56" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="96" priority="13">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="beginsWith" dxfId="55" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="95" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="54" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="94" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="53" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="93" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B13">
-    <cfRule type="expression" dxfId="52" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="51" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="91" priority="8">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="50" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="90" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="49" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="89" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="48" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="88" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4968,8 +6597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15D721F-E928-8949-A67C-84C364E740E7}">
   <dimension ref="A1:AAA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A21" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -4986,7 +6615,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
@@ -5009,16 +6638,16 @@
         <v>255</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>281</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>284</v>
       </c>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
@@ -5035,27 +6664,27 @@
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>253</v>
+        <v>289</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>0</v>
+        <v>209</v>
       </c>
       <c r="HA5" s="6"/>
       <c r="AAA5" s="6"/>
     </row>
     <row r="6" spans="1:703" ht="23" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="HA6" s="6"/>
       <c r="AAA6" s="6"/>
     </row>
     <row r="7" spans="1:703" ht="23" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
@@ -5065,7 +6694,7 @@
     </row>
     <row r="8" spans="1:703" ht="23" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
@@ -5075,281 +6704,279 @@
     </row>
     <row r="9" spans="1:703" ht="23" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>267</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>0</v>
+        <v>194</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>283</v>
       </c>
       <c r="HA9" s="6"/>
       <c r="AAA9" s="6"/>
     </row>
     <row r="10" spans="1:703" ht="23" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>265</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>194</v>
+        <v>290</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="HA10" s="6"/>
       <c r="AAA10" s="6"/>
     </row>
     <row r="11" spans="1:703" ht="23" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>287</v>
+        <v>0</v>
       </c>
       <c r="HA11" s="6"/>
       <c r="AAA11" s="6"/>
     </row>
     <row r="12" spans="1:703" ht="23" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>0</v>
+        <v>292</v>
       </c>
       <c r="HA12" s="6"/>
       <c r="AAA12" s="6"/>
     </row>
     <row r="13" spans="1:703" ht="23" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="HA13" s="6"/>
       <c r="AAA13" s="6"/>
     </row>
     <row r="14" spans="1:703" ht="23" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>269</v>
+        <v>196</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>270</v>
+        <v>195</v>
       </c>
       <c r="HA14" s="6"/>
       <c r="AAA14" s="6"/>
     </row>
     <row r="15" spans="1:703" ht="23" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="HA15" s="6"/>
       <c r="AAA15" s="6"/>
     </row>
     <row r="16" spans="1:703" ht="23" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="HA16" s="6"/>
       <c r="AAA16" s="6"/>
     </row>
     <row r="17" spans="1:703" ht="23" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="HA17" s="6"/>
-      <c r="AAA17" s="6"/>
+        <v>202</v>
+      </c>
+      <c r="HA17" s="4"/>
+      <c r="AAA17" s="5"/>
     </row>
     <row r="18" spans="1:703" ht="23" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="HA18" s="4"/>
       <c r="AAA18" s="5"/>
     </row>
     <row r="19" spans="1:703" ht="23" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="HA19" s="4"/>
       <c r="AAA19" s="5"/>
     </row>
     <row r="20" spans="1:703" ht="23" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="HA20" s="4"/>
       <c r="AAA20" s="5"/>
     </row>
     <row r="21" spans="1:703" ht="23" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="HA21" s="4"/>
       <c r="AAA21" s="5"/>
     </row>
     <row r="22" spans="1:703" ht="23" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="HA22" s="4"/>
       <c r="AAA22" s="5"/>
     </row>
     <row r="23" spans="1:703" ht="23" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="HA23" s="4"/>
       <c r="AAA23" s="5"/>
     </row>
     <row r="24" spans="1:703" ht="23" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="HA24" s="4"/>
       <c r="AAA24" s="5"/>
     </row>
     <row r="25" spans="1:703" ht="23" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>212</v>
+        <v>269</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>217</v>
+        <v>270</v>
       </c>
       <c r="HA25" s="4"/>
       <c r="AAA25" s="5"/>
     </row>
     <row r="26" spans="1:703" ht="23" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>271</v>
+        <v>214</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="HA26" s="4"/>
-      <c r="AAA26" s="5"/>
+        <v>276</v>
+      </c>
     </row>
     <row r="27" spans="1:703" ht="23" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>278</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:703" ht="23" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>218</v>
+        <v>247</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>219</v>
+        <v>246</v>
       </c>
     </row>
     <row r="29" spans="1:703" ht="23" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>247</v>
+        <v>271</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>246</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:703" ht="23" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>273</v>
+        <v>220</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>279</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:703" ht="23" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>234</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="1:703" ht="23" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="23" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="23" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="23" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="23" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="23" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>226</v>
+        <v>260</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>230</v>
+        <v>261</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="23" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>262</v>
@@ -5357,90 +6984,90 @@
     </row>
     <row r="39" spans="1:2" ht="23" customHeight="1">
       <c r="A39" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="23" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>265</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="23" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="23" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="23" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>238</v>
+        <v>284</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>239</v>
+        <v>285</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="23" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>289</v>
+        <v>243</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="23" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="23" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="23" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="23" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>250</v>
+        <v>287</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>251</v>
+        <v>288</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="23" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="23" customHeight="1">
@@ -5453,10 +7080,10 @@
     </row>
     <row r="51" spans="1:2" ht="23" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="23" customHeight="1">
@@ -5477,195 +7104,176 @@
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <sortState ref="A2:B7">
-    <sortCondition ref="A2:A7"/>
+  <sortState ref="A2:B8">
+    <sortCondition ref="A2:A8"/>
   </sortState>
-  <conditionalFormatting sqref="A35:A49 A54:A1048576 A31:A32">
-    <cfRule type="beginsWith" dxfId="47" priority="55" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A31,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="56" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A31,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="45" priority="57" stopIfTrue="1">
-      <formula>LEN(TRIM(A31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B54:B1048576 B29:B32 B35:B49">
-    <cfRule type="expression" dxfId="44" priority="58" stopIfTrue="1">
+  <conditionalFormatting sqref="A34:A49 A54:A1048576 A30:A31 A7:A13">
+    <cfRule type="beginsWith" dxfId="87" priority="55" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A7,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="86" priority="56" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A7,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="85" priority="57" stopIfTrue="1">
+      <formula>LEN(TRIM(A7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54:B1048576 B28:B31 B34:B49 B7:B13">
+    <cfRule type="expression" dxfId="84" priority="58" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="43" priority="59">
-      <formula>LEN(TRIM(B29))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15:A23 A25:A30">
-    <cfRule type="beginsWith" dxfId="42" priority="50" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="41" priority="51" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="40" priority="52" stopIfTrue="1">
-      <formula>LEN(TRIM(A15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:B23 B25:B27 B29:B30">
-    <cfRule type="expression" dxfId="39" priority="53" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="59">
+      <formula>LEN(TRIM(B7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:A22 A24:A29">
+    <cfRule type="beginsWith" dxfId="82" priority="50" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="81" priority="51" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="80" priority="52" stopIfTrue="1">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:B22 B24:B26 B28:B29">
+    <cfRule type="expression" dxfId="79" priority="53" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="38" priority="54">
-      <formula>LEN(TRIM(B15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
-    <cfRule type="beginsWith" dxfId="37" priority="42" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A24,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="36" priority="43" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A24,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="35" priority="44" stopIfTrue="1">
-      <formula>LEN(TRIM(A24))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="34" priority="45" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="54">
+      <formula>LEN(TRIM(B14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="beginsWith" dxfId="77" priority="42" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A23,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="76" priority="43" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A23,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="75" priority="44" stopIfTrue="1">
+      <formula>LEN(TRIM(A23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23">
+    <cfRule type="expression" dxfId="74" priority="45" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="33" priority="46">
-      <formula>LEN(TRIM(B24))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="32" priority="40" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="46">
+      <formula>LEN(TRIM(B23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="expression" dxfId="72" priority="40" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="31" priority="41">
-      <formula>LEN(TRIM(B28))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33:A34">
-    <cfRule type="beginsWith" dxfId="30" priority="35" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A33,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="29" priority="36" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A33,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="28" priority="37" stopIfTrue="1">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33:B34">
-    <cfRule type="expression" dxfId="27" priority="38" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="41">
+      <formula>LEN(TRIM(B27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32:A33">
+    <cfRule type="beginsWith" dxfId="70" priority="35" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A32,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="69" priority="36" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A32,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="68" priority="37" stopIfTrue="1">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:B33">
+    <cfRule type="expression" dxfId="67" priority="38" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="26" priority="39">
-      <formula>LEN(TRIM(B33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A5">
-    <cfRule type="beginsWith" dxfId="25" priority="25" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="39">
+      <formula>LEN(TRIM(B32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A6">
+    <cfRule type="beginsWith" dxfId="65" priority="25" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="64" priority="26" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="23" priority="27" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="27" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B5">
-    <cfRule type="expression" dxfId="22" priority="28" stopIfTrue="1">
+  <conditionalFormatting sqref="B2:B6">
+    <cfRule type="expression" dxfId="62" priority="28" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="21" priority="29">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="29">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:A14">
-    <cfRule type="beginsWith" dxfId="20" priority="20" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A6,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="21" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A6,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="22" stopIfTrue="1">
-      <formula>LEN(TRIM(A6))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6:B14">
-    <cfRule type="expression" dxfId="17" priority="23" stopIfTrue="1">
+  <conditionalFormatting sqref="A52:A53">
+    <cfRule type="beginsWith" dxfId="60" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A52,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="59" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A52,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="58" priority="17" stopIfTrue="1">
+      <formula>LEN(TRIM(A52))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50:B51 B53">
+    <cfRule type="expression" dxfId="57" priority="18" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="16" priority="24">
-      <formula>LEN(TRIM(B6))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52:A53">
-    <cfRule type="beginsWith" dxfId="15" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A52,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A52,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="13" priority="17" stopIfTrue="1">
-      <formula>LEN(TRIM(A52))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B50:B51 B53">
-    <cfRule type="expression" dxfId="12" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="19">
+      <formula>LEN(TRIM(B50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="beginsWith" dxfId="55" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A50,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="54" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A50,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="53" priority="12" stopIfTrue="1">
+      <formula>LEN(TRIM(A50))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50">
+    <cfRule type="expression" dxfId="52" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="11" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="14">
       <formula>LEN(TRIM(B50))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A50">
-    <cfRule type="beginsWith" dxfId="10" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
-      <formula>LEFT(A50,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="9" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.">
-      <formula>LEFT(A50,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="8" priority="12" stopIfTrue="1">
-      <formula>LEN(TRIM(A50))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B50">
-    <cfRule type="expression" dxfId="7" priority="13" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="6" priority="14">
-      <formula>LEN(TRIM(B50))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="beginsWith" dxfId="5" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="50" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A51,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="49" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A51,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="9" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="9" stopIfTrue="1">
       <formula>LEN(TRIM(A51))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="47" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="46" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="B13 B22 B50 B52:B53" numberStoredAsText="1"/>
+    <ignoredError sqref="B21 B50 B52:B53" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed web-03 and web-04
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-03.data.xlsx
+++ b/artifact/data/web-03.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8446527-20CE-8E41-BD2E-066E4805A82D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300F0D14-1672-984D-8F07-854F84BC9FDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="15780" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="32000" windowHeight="8780" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -4426,7 +4426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03856218-1A13-8840-A44A-29262810A7AA}">
   <dimension ref="A1:AAA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -6597,8 +6597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15D721F-E928-8949-A67C-84C364E740E7}">
   <dimension ref="A1:AAA53"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -6615,7 +6615,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>282</v>
+        <v>119</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>

</xml_diff>

<commit_message>
- code fix for downloading electron driver
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-03.data.xlsx
+++ b/artifact/data/web-03.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE2E4AA-6678-004E-91D6-FC45D458B366}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF018310-2281-C841-9427-BA1835E94E79}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="34600" windowHeight="17620" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="6840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -4224,7 +4224,7 @@
   <dimension ref="A1:AAA21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -5111,7 +5111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02992098-561F-1944-A340-34CB95735B3B}">
   <dimension ref="A1:AAA9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" zoomScale="139" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -5363,7 +5363,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17A18B9-A7F4-B848-8E0C-853951D12261}">
   <dimension ref="A1:AAA8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -6295,7 +6297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938A5DF5-858F-F04F-A650-D78F3893CC59}">
   <dimension ref="A1:AAA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>

</xml_diff>